<commit_message>
Corrected version of line of thrust calcs. Reverted to a simpler method for computing side forces from Q and solving for line of thrust using moments about center of base.
</commit_message>
<xml_diff>
--- a/thrust_calc_resuls.xlsx
+++ b/thrust_calc_resuls.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:U21"/>
+  <dimension ref="A1:AC21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -441,27 +441,27 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>alpha (deg)</t>
+          <t>N_eff</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>alpha (rad)</t>
+          <t>dl</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>N_eff'</t>
+          <t>dx</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>dl</t>
+          <t>y_lb</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>dx</t>
+          <t>y_rb</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
@@ -476,7 +476,7 @@
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>cm</t>
+          <t>c_m</t>
         </is>
       </c>
       <c r="J1" s="1" t="inlineStr">
@@ -486,57 +486,97 @@
       </c>
       <c r="K1" s="1" t="inlineStr">
         <is>
+          <t>Q</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
           <t>Z_left</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="M1" s="1" t="inlineStr">
         <is>
           <t>Z_right</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="N1" s="1" t="inlineStr">
         <is>
           <t>X_left</t>
         </is>
       </c>
-      <c r="N1" s="1" t="inlineStr">
+      <c r="O1" s="1" t="inlineStr">
         <is>
           <t>X_right</t>
         </is>
       </c>
-      <c r="O1" s="1" t="inlineStr">
+      <c r="P1" s="1" t="inlineStr">
         <is>
           <t>E_left</t>
         </is>
       </c>
-      <c r="P1" s="1" t="inlineStr">
+      <c r="Q1" s="1" t="inlineStr">
         <is>
           <t>E_right</t>
         </is>
       </c>
-      <c r="Q1" s="1" t="inlineStr">
-        <is>
-          <t>delta_y_left</t>
-        </is>
-      </c>
       <c r="R1" s="1" t="inlineStr">
         <is>
-          <t>delta_y_right</t>
+          <t>delta_y_L</t>
         </is>
       </c>
       <c r="S1" s="1" t="inlineStr">
         <is>
+          <t>delta_y_R</t>
+        </is>
+      </c>
+      <c r="T1" s="1" t="inlineStr">
+        <is>
+          <t>y_L_abs_left</t>
+        </is>
+      </c>
+      <c r="U1" s="1" t="inlineStr">
+        <is>
+          <t>y_L_abs_right</t>
+        </is>
+      </c>
+      <c r="V1" s="1" t="inlineStr">
+        <is>
+          <t>y_R_abs_left</t>
+        </is>
+      </c>
+      <c r="W1" s="1" t="inlineStr">
+        <is>
+          <t>y_R_abs_right</t>
+        </is>
+      </c>
+      <c r="X1" s="1" t="inlineStr">
+        <is>
+          <t>y_ave_left</t>
+        </is>
+      </c>
+      <c r="Y1" s="1" t="inlineStr">
+        <is>
+          <t>y_ave_right</t>
+        </is>
+      </c>
+      <c r="Z1" s="1" t="inlineStr">
+        <is>
           <t>fx_residual</t>
         </is>
       </c>
-      <c r="T1" s="1" t="inlineStr">
+      <c r="AA1" s="1" t="inlineStr">
         <is>
           <t>fy_residual</t>
         </is>
       </c>
-      <c r="U1" s="1" t="inlineStr">
-        <is>
-          <t>moment_residual</t>
+      <c r="AB1" s="1" t="inlineStr">
+        <is>
+          <t>moment_residual_L</t>
+        </is>
+      </c>
+      <c r="AC1" s="1" t="inlineStr">
+        <is>
+          <t>moment_residual_R</t>
         </is>
       </c>
     </row>
@@ -545,64 +585,88 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>-44.71555019038</v>
+        <v>237.7093179607289</v>
       </c>
       <c r="C2" t="n">
-        <v>-0.7804335776629082</v>
+        <v>3.002649017626326</v>
       </c>
       <c r="D2" t="n">
-        <v>17126.73162235983</v>
+        <v>2.932944702391879</v>
       </c>
       <c r="E2" t="n">
-        <v>14.10583813984129</v>
+        <v>40.2112427661442</v>
       </c>
       <c r="F2" t="n">
-        <v>10.02372911589109</v>
+        <v>40.8545666849556</v>
       </c>
       <c r="G2" t="n">
-        <v>329.0368204760222</v>
+        <v>55.45844653925082</v>
       </c>
       <c r="H2" t="n">
-        <v>6976.910679550587</v>
+        <v>312.8010711157287</v>
       </c>
       <c r="I2" t="n">
-        <v>207.6712460492573</v>
+        <v>118.0287782037461</v>
       </c>
       <c r="J2" t="n">
-        <v>0.2645344624757899</v>
+        <v>0.7375256614282456</v>
       </c>
       <c r="K2" t="n">
-        <v>0</v>
+        <v>-473.1159324358758</v>
       </c>
       <c r="L2" t="n">
-        <v>20870.36326315546</v>
+        <v>0</v>
       </c>
       <c r="M2" t="n">
-        <v>0</v>
+        <v>473.1159324358759</v>
       </c>
       <c r="N2" t="n">
-        <v>20616.87615337185</v>
+        <v>0</v>
       </c>
       <c r="O2" t="n">
-        <v>0</v>
+        <v>195.5215581771053</v>
       </c>
       <c r="P2" t="n">
-        <v>3242.912335015561</v>
+        <v>0</v>
       </c>
       <c r="Q2" t="n">
-        <v>0</v>
+        <v>430.8247971190436</v>
       </c>
       <c r="R2" t="n">
-        <v>31.86302317609248</v>
+        <v>0</v>
       </c>
       <c r="S2" t="n">
-        <v>9.094947017729282e-13</v>
+        <v>0</v>
       </c>
       <c r="T2" t="n">
-        <v>-1.818989403545856e-12</v>
+        <v>40.2112427661442</v>
       </c>
       <c r="U2" t="n">
-        <v>0</v>
+        <v>41.1984852314757</v>
+      </c>
+      <c r="V2" t="n">
+        <v>40.2112427661442</v>
+      </c>
+      <c r="W2" t="n">
+        <v>41.24132833289816</v>
+      </c>
+      <c r="X2" t="n">
+        <v>40.2112427661442</v>
+      </c>
+      <c r="Y2" t="n">
+        <v>41.21990678218693</v>
+      </c>
+      <c r="Z2" t="n">
+        <v>5.684341886080801e-14</v>
+      </c>
+      <c r="AA2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC2" t="n">
+        <v>18.50112508308393</v>
       </c>
     </row>
     <row r="3">
@@ -610,63 +674,87 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>-38.32026139738871</v>
+        <v>476.7265339988375</v>
       </c>
       <c r="C3" t="n">
-        <v>-0.668814731609316</v>
+        <v>3.02746902981108</v>
       </c>
       <c r="D3" t="n">
-        <v>26393.52910615979</v>
+        <v>2.932944702391893</v>
       </c>
       <c r="E3" t="n">
-        <v>12.77628929067389</v>
+        <v>40.8545666849556</v>
       </c>
       <c r="F3" t="n">
-        <v>10.02372911589107</v>
+        <v>41.60529025955755</v>
       </c>
       <c r="G3" t="n">
-        <v>882.7639613190732</v>
+        <v>160.3760130791467</v>
       </c>
       <c r="H3" t="n">
-        <v>18718.16443016667</v>
+        <v>904.5653422138773</v>
       </c>
       <c r="I3" t="n">
-        <v>207.6712460492573</v>
+        <v>118.0287782037461</v>
       </c>
       <c r="J3" t="n">
-        <v>0.2645344624757899</v>
+        <v>0.7375256614282456</v>
       </c>
       <c r="K3" t="n">
-        <v>20870.36326315546</v>
+        <v>-492.2170383978711</v>
       </c>
       <c r="L3" t="n">
-        <v>52168.67746883236</v>
+        <v>473.1159324358759</v>
       </c>
       <c r="M3" t="n">
-        <v>20616.87615337185</v>
+        <v>965.3329708337468</v>
       </c>
       <c r="N3" t="n">
-        <v>51535.04751682509</v>
+        <v>195.5215581771053</v>
       </c>
       <c r="O3" t="n">
-        <v>3242.912335015561</v>
+        <v>398.9369067437394</v>
       </c>
       <c r="P3" t="n">
-        <v>8106.157306988158</v>
+        <v>430.8247971190436</v>
       </c>
       <c r="Q3" t="n">
-        <v>31.86302317609248</v>
+        <v>879.0432805137893</v>
       </c>
       <c r="R3" t="n">
-        <v>57.35697474289933</v>
+        <v>0.3439185465200971</v>
       </c>
       <c r="S3" t="n">
-        <v>0</v>
+        <v>0.3867616479425661</v>
       </c>
       <c r="T3" t="n">
-        <v>-5.456968210637569e-12</v>
+        <v>41.1984852314757</v>
       </c>
       <c r="U3" t="n">
+        <v>42.20625982014061</v>
+      </c>
+      <c r="V3" t="n">
+        <v>41.24132833289816</v>
+      </c>
+      <c r="W3" t="n">
+        <v>42.2271957613879</v>
+      </c>
+      <c r="X3" t="n">
+        <v>41.21990678218693</v>
+      </c>
+      <c r="Y3" t="n">
+        <v>42.21672779076425</v>
+      </c>
+      <c r="Z3" t="n">
+        <v>-1.13686837721616e-13</v>
+      </c>
+      <c r="AA3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC3" t="n">
         <v>0</v>
       </c>
     </row>
@@ -675,63 +763,87 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>-32.44742192315573</v>
+        <v>671.8958345871947</v>
       </c>
       <c r="C4" t="n">
-        <v>-0.566314346342858</v>
+        <v>3.056681131130836</v>
       </c>
       <c r="D4" t="n">
-        <v>30590.57201577538</v>
+        <v>2.932944702391879</v>
       </c>
       <c r="E4" t="n">
-        <v>11.87808673064982</v>
+        <v>41.60529025955755</v>
       </c>
       <c r="F4" t="n">
-        <v>10.02372911589109</v>
+        <v>42.46632650231609</v>
       </c>
       <c r="G4" t="n">
-        <v>1327.004522339517</v>
+        <v>258.5050573845721</v>
       </c>
       <c r="H4" t="n">
-        <v>28137.86010431374</v>
+        <v>1458.040458841518</v>
       </c>
       <c r="I4" t="n">
-        <v>207.6712460492573</v>
+        <v>118.0287782037461</v>
       </c>
       <c r="J4" t="n">
-        <v>0.2645344624757899</v>
+        <v>0.7375256614282456</v>
       </c>
       <c r="K4" t="n">
-        <v>52168.67746883236</v>
+        <v>-450.107471870699</v>
       </c>
       <c r="L4" t="n">
-        <v>86364.05951491567</v>
+        <v>965.3329708337468</v>
       </c>
       <c r="M4" t="n">
-        <v>51535.04751682509</v>
+        <v>1415.440442704446</v>
       </c>
       <c r="N4" t="n">
-        <v>85315.09953469991</v>
+        <v>398.9369067437394</v>
       </c>
       <c r="O4" t="n">
-        <v>8106.157306988158</v>
+        <v>584.949907392887</v>
       </c>
       <c r="P4" t="n">
-        <v>13419.55913136287</v>
+        <v>879.0432805137893</v>
       </c>
       <c r="Q4" t="n">
-        <v>57.35697474289933</v>
+        <v>1288.916309418269</v>
       </c>
       <c r="R4" t="n">
-        <v>85.75684569148636</v>
+        <v>0.6009695605830594</v>
       </c>
       <c r="S4" t="n">
-        <v>-7.275957614183426e-12</v>
+        <v>0.6219055018303444</v>
       </c>
       <c r="T4" t="n">
-        <v>5.456968210637569e-12</v>
+        <v>42.20625982014061</v>
       </c>
       <c r="U4" t="n">
+        <v>43.27150271255194</v>
+      </c>
+      <c r="V4" t="n">
+        <v>42.2271957613879</v>
+      </c>
+      <c r="W4" t="n">
+        <v>43.28573517065568</v>
+      </c>
+      <c r="X4" t="n">
+        <v>42.21672779076425</v>
+      </c>
+      <c r="Y4" t="n">
+        <v>43.27861894160381</v>
+      </c>
+      <c r="Z4" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA4" t="n">
+        <v>-5.684341886080801e-14</v>
+      </c>
+      <c r="AB4" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC4" t="n">
         <v>0</v>
       </c>
     </row>
@@ -740,63 +852,87 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>-26.9359618041506</v>
+        <v>828.1881288838915</v>
       </c>
       <c r="C5" t="n">
-        <v>-0.4701212206738599</v>
+        <v>3.090648533113749</v>
       </c>
       <c r="D5" t="n">
-        <v>32499.18525670047</v>
+        <v>2.932944702391893</v>
       </c>
       <c r="E5" t="n">
-        <v>11.24349820547246</v>
+        <v>42.46632650231609</v>
       </c>
       <c r="F5" t="n">
-        <v>10.02372911589107</v>
+        <v>43.44114784283002</v>
       </c>
       <c r="G5" t="n">
-        <v>1683.652215421597</v>
+        <v>349.6468918888771</v>
       </c>
       <c r="H5" t="n">
-        <v>35700.23289621456</v>
+        <v>1972.105767833217</v>
       </c>
       <c r="I5" t="n">
-        <v>207.6712460492573</v>
+        <v>118.0287782037461</v>
       </c>
       <c r="J5" t="n">
-        <v>0.2645344624757899</v>
+        <v>0.7375256614282456</v>
       </c>
       <c r="K5" t="n">
-        <v>86364.05951491567</v>
+        <v>-355.6489776896068</v>
       </c>
       <c r="L5" t="n">
-        <v>119813.6443566896</v>
+        <v>1415.440442704446</v>
       </c>
       <c r="M5" t="n">
-        <v>85315.09953469991</v>
+        <v>1771.089420394052</v>
       </c>
       <c r="N5" t="n">
-        <v>118358.4126466486</v>
+        <v>584.949907392887</v>
       </c>
       <c r="O5" t="n">
-        <v>13419.55913136287</v>
+        <v>731.9266577296371</v>
       </c>
       <c r="P5" t="n">
-        <v>18617.0762956203</v>
+        <v>1288.916309418269</v>
       </c>
       <c r="Q5" t="n">
-        <v>85.75684569148636</v>
+        <v>1612.774349602716</v>
       </c>
       <c r="R5" t="n">
-        <v>116.6457656555302</v>
+        <v>0.8051762102358407</v>
       </c>
       <c r="S5" t="n">
-        <v>0</v>
+        <v>0.8194086683395876</v>
       </c>
       <c r="T5" t="n">
-        <v>0</v>
+        <v>43.27150271255194</v>
       </c>
       <c r="U5" t="n">
+        <v>44.40512676931859</v>
+      </c>
+      <c r="V5" t="n">
+        <v>43.28573517065568</v>
+      </c>
+      <c r="W5" t="n">
+        <v>44.41646694287392</v>
+      </c>
+      <c r="X5" t="n">
+        <v>43.27861894160381</v>
+      </c>
+      <c r="Y5" t="n">
+        <v>44.41079685609625</v>
+      </c>
+      <c r="Z5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC5" t="n">
         <v>0</v>
       </c>
     </row>
@@ -805,63 +941,87 @@
         <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>-21.68252031424755</v>
+        <v>949.6680916848178</v>
       </c>
       <c r="C6" t="n">
-        <v>-0.3784313696141753</v>
+        <v>3.129816832228253</v>
       </c>
       <c r="D6" t="n">
-        <v>33169.00469766767</v>
+        <v>2.932944702391865</v>
       </c>
       <c r="E6" t="n">
-        <v>10.78695667671407</v>
+        <v>43.44114784283002</v>
       </c>
       <c r="F6" t="n">
-        <v>10.02372911589109</v>
+        <v>44.53386404841829</v>
       </c>
       <c r="G6" t="n">
-        <v>1966.189034868296</v>
+        <v>433.5656336917605</v>
       </c>
       <c r="H6" t="n">
-        <v>41691.15558417432</v>
+        <v>2445.430823991193</v>
       </c>
       <c r="I6" t="n">
-        <v>207.6712460492573</v>
+        <v>118.0287782037461</v>
       </c>
       <c r="J6" t="n">
-        <v>0.2645344624757899</v>
+        <v>0.7375256614282456</v>
       </c>
       <c r="K6" t="n">
-        <v>119813.6443566896</v>
+        <v>-216.7171224627084</v>
       </c>
       <c r="L6" t="n">
-        <v>150512.4129945929</v>
+        <v>1771.089420394052</v>
       </c>
       <c r="M6" t="n">
-        <v>118358.4126466486</v>
+        <v>1987.80654285676</v>
       </c>
       <c r="N6" t="n">
-        <v>148684.320398624</v>
+        <v>731.9266577296371</v>
       </c>
       <c r="O6" t="n">
-        <v>18617.0762956203</v>
+        <v>821.4879397803325</v>
       </c>
       <c r="P6" t="n">
-        <v>23387.1617143728</v>
+        <v>1612.774349602716</v>
       </c>
       <c r="Q6" t="n">
-        <v>116.6457656555302</v>
+        <v>1810.119448163466</v>
       </c>
       <c r="R6" t="n">
-        <v>150.0817059737297</v>
+        <v>0.9639789264885716</v>
       </c>
       <c r="S6" t="n">
-        <v>2.91038304567337e-11</v>
+        <v>0.9753191000438998</v>
       </c>
       <c r="T6" t="n">
-        <v>0</v>
+        <v>44.40512676931859</v>
       </c>
       <c r="U6" t="n">
+        <v>45.61810970341703</v>
+      </c>
+      <c r="V6" t="n">
+        <v>44.41646694287392</v>
+      </c>
+      <c r="W6" t="n">
+        <v>45.62819158591584</v>
+      </c>
+      <c r="X6" t="n">
+        <v>44.41079685609625</v>
+      </c>
+      <c r="Y6" t="n">
+        <v>45.62315064466644</v>
+      </c>
+      <c r="Z6" t="n">
+        <v>2.273736754432321e-13</v>
+      </c>
+      <c r="AA6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC6" t="n">
         <v>0</v>
       </c>
     </row>
@@ -870,64 +1030,88 @@
         <v>5</v>
       </c>
       <c r="B7" t="n">
-        <v>-16.61457905447066</v>
+        <v>1153.27459322714</v>
       </c>
       <c r="C7" t="n">
-        <v>-0.2899791083333994</v>
+        <v>3.174732126033935</v>
       </c>
       <c r="D7" t="n">
-        <v>33075.71777992717</v>
+        <v>2.932944702391893</v>
       </c>
       <c r="E7" t="n">
-        <v>10.46045467471967</v>
+        <v>44.53386404841829</v>
       </c>
       <c r="F7" t="n">
-        <v>10.02372911589109</v>
+        <v>45.74932103578577</v>
       </c>
       <c r="G7" t="n">
-        <v>2183.374874140138</v>
+        <v>475.0732646157159</v>
       </c>
       <c r="H7" t="n">
-        <v>46296.37332020365</v>
+        <v>2876.444518868235</v>
       </c>
       <c r="I7" t="n">
-        <v>207.6712460492573</v>
+        <v>118.0287782037461</v>
       </c>
       <c r="J7" t="n">
-        <v>0.2645344624757899</v>
+        <v>0.7375256614282456</v>
       </c>
       <c r="K7" t="n">
-        <v>150512.4129945929</v>
+        <v>-124.3062317733032</v>
       </c>
       <c r="L7" t="n">
-        <v>177291.5195301109</v>
+        <v>1987.80654285676</v>
       </c>
       <c r="M7" t="n">
-        <v>148684.320398624</v>
+        <v>2112.112774630063</v>
       </c>
       <c r="N7" t="n">
-        <v>175138.1734523178</v>
+        <v>821.4879397803325</v>
       </c>
       <c r="O7" t="n">
-        <v>23387.1617143728</v>
+        <v>872.8591713562944</v>
       </c>
       <c r="P7" t="n">
-        <v>27548.19589522188</v>
+        <v>1810.119448163466</v>
       </c>
       <c r="Q7" t="n">
-        <v>150.0817059737297</v>
+        <v>1923.314129240127</v>
       </c>
       <c r="R7" t="n">
-        <v>186.3257988834008</v>
+        <v>1.084245654998742</v>
       </c>
       <c r="S7" t="n">
-        <v>0</v>
+        <v>1.094327537497543</v>
       </c>
       <c r="T7" t="n">
-        <v>0</v>
+        <v>45.61810970341703</v>
       </c>
       <c r="U7" t="n">
-        <v>0</v>
+        <v>46.8819632592918</v>
+      </c>
+      <c r="V7" t="n">
+        <v>45.62819158591584</v>
+      </c>
+      <c r="W7" t="n">
+        <v>46.89143783035405</v>
+      </c>
+      <c r="X7" t="n">
+        <v>45.62315064466644</v>
+      </c>
+      <c r="Y7" t="n">
+        <v>46.88670054482293</v>
+      </c>
+      <c r="Z7" t="n">
+        <v>2.273736754432321e-13</v>
+      </c>
+      <c r="AA7" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB7" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC7" t="n">
+        <v>9.094947017729282e-13</v>
       </c>
     </row>
     <row r="8">
@@ -935,63 +1119,87 @@
         <v>6</v>
       </c>
       <c r="B8" t="n">
-        <v>-11.71569679076375</v>
+        <v>1418.884452919824</v>
       </c>
       <c r="C8" t="n">
-        <v>-0.2044774831641606</v>
+        <v>3.226065103393914</v>
       </c>
       <c r="D8" t="n">
-        <v>34936.28971150933</v>
+        <v>2.932944702391893</v>
       </c>
       <c r="E8" t="n">
-        <v>10.07659006958534</v>
+        <v>45.74932103578577</v>
       </c>
       <c r="F8" t="n">
-        <v>9.866666666666674</v>
+        <v>47.09322675736657</v>
       </c>
       <c r="G8" t="n">
-        <v>2589.604130495291</v>
+        <v>479.7382027375878</v>
       </c>
       <c r="H8" t="n">
-        <v>53576.08621085047</v>
+        <v>3263.29585778987</v>
       </c>
       <c r="I8" t="n">
-        <v>51.91781151231434</v>
+        <v>118.0287782037461</v>
       </c>
       <c r="J8" t="n">
-        <v>0.3244184923225048</v>
+        <v>0.7375256614282456</v>
       </c>
       <c r="K8" t="n">
-        <v>177291.5195301109</v>
+        <v>-68.10015948106651</v>
       </c>
       <c r="L8" t="n">
-        <v>201589.3684865372</v>
+        <v>2112.112774630063</v>
       </c>
       <c r="M8" t="n">
-        <v>175138.1734523178</v>
+        <v>2180.212934111129</v>
       </c>
       <c r="N8" t="n">
-        <v>199140.9057675884</v>
+        <v>872.8591713562944</v>
       </c>
       <c r="O8" t="n">
-        <v>27548.19589522188</v>
+        <v>901.0024833460087</v>
       </c>
       <c r="P8" t="n">
-        <v>31323.68332213438</v>
+        <v>1923.314129240127</v>
       </c>
       <c r="Q8" t="n">
-        <v>186.3257988834008</v>
+        <v>1985.326915918329</v>
       </c>
       <c r="R8" t="n">
-        <v>222.8148903716774</v>
+        <v>1.132642223506032</v>
       </c>
       <c r="S8" t="n">
-        <v>-2.91038304567337e-11</v>
+        <v>1.142116794568282</v>
       </c>
       <c r="T8" t="n">
-        <v>0</v>
+        <v>46.8819632592918</v>
       </c>
       <c r="U8" t="n">
+        <v>48.17785014116642</v>
+      </c>
+      <c r="V8" t="n">
+        <v>46.89143783035405</v>
+      </c>
+      <c r="W8" t="n">
+        <v>48.18702003842085</v>
+      </c>
+      <c r="X8" t="n">
+        <v>46.88670054482293</v>
+      </c>
+      <c r="Y8" t="n">
+        <v>48.18243508979364</v>
+      </c>
+      <c r="Z8" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA8" t="n">
+        <v>1.13686837721616e-13</v>
+      </c>
+      <c r="AB8" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC8" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1000,63 +1208,87 @@
         <v>7</v>
       </c>
       <c r="B9" t="n">
-        <v>-6.940199065150054</v>
+        <v>1654.425575982639</v>
       </c>
       <c r="C9" t="n">
-        <v>-0.1211293244307009</v>
+        <v>3.284643417092181</v>
       </c>
       <c r="D9" t="n">
-        <v>38956.74174810763</v>
+        <v>2.932944702391893</v>
       </c>
       <c r="E9" t="n">
-        <v>9.939495248171937</v>
+        <v>47.09322675736657</v>
       </c>
       <c r="F9" t="n">
-        <v>9.866666666666674</v>
+        <v>48.57231281173381</v>
       </c>
       <c r="G9" t="n">
-        <v>3189.933993141789</v>
+        <v>476.1866347544442</v>
       </c>
       <c r="H9" t="n">
-        <v>65158.84795942099</v>
+        <v>3603.803815840586</v>
       </c>
       <c r="I9" t="n">
-        <v>51.91781151231434</v>
+        <v>118.0287782037461</v>
       </c>
       <c r="J9" t="n">
-        <v>0.3244184923225048</v>
+        <v>0.7375256614282456</v>
       </c>
       <c r="K9" t="n">
-        <v>201589.3684865372</v>
+        <v>14.59082993173172</v>
       </c>
       <c r="L9" t="n">
-        <v>223451.2939094523</v>
+        <v>2180.212934111129</v>
       </c>
       <c r="M9" t="n">
-        <v>199140.9057675884</v>
+        <v>2165.622104179397</v>
       </c>
       <c r="N9" t="n">
-        <v>220737.3007720875</v>
+        <v>901.0024833460087</v>
       </c>
       <c r="O9" t="n">
-        <v>31323.68332213438</v>
+        <v>894.9726255294235</v>
       </c>
       <c r="P9" t="n">
-        <v>34720.66816265808</v>
+        <v>1985.326915918329</v>
       </c>
       <c r="Q9" t="n">
-        <v>222.8148903716774</v>
+        <v>1972.040338751561</v>
       </c>
       <c r="R9" t="n">
-        <v>260.6741948432603</v>
+        <v>1.084623383799854</v>
       </c>
       <c r="S9" t="n">
-        <v>0</v>
+        <v>1.093793281054288</v>
       </c>
       <c r="T9" t="n">
-        <v>0</v>
+        <v>48.17785014116642</v>
       </c>
       <c r="U9" t="n">
+        <v>49.51571860632898</v>
+      </c>
+      <c r="V9" t="n">
+        <v>48.18702003842085</v>
+      </c>
+      <c r="W9" t="n">
+        <v>49.52495251284039</v>
+      </c>
+      <c r="X9" t="n">
+        <v>48.18243508979364</v>
+      </c>
+      <c r="Y9" t="n">
+        <v>49.52033555958468</v>
+      </c>
+      <c r="Z9" t="n">
+        <v>4.547473508864641e-13</v>
+      </c>
+      <c r="AA9" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB9" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC9" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1065,63 +1297,87 @@
         <v>8</v>
       </c>
       <c r="B10" t="n">
-        <v>-2.212803763689251</v>
+        <v>1863.095327594637</v>
       </c>
       <c r="C10" t="n">
-        <v>-0.03862071137689997</v>
+        <v>3.351495771472501</v>
       </c>
       <c r="D10" t="n">
-        <v>44324.77245843505</v>
+        <v>2.932944702391865</v>
       </c>
       <c r="E10" t="n">
-        <v>9.874029601984471</v>
+        <v>48.57231281173381</v>
       </c>
       <c r="F10" t="n">
-        <v>9.866666666666674</v>
+        <v>50.19454407086326</v>
       </c>
       <c r="G10" t="n">
-        <v>3523.376295930079</v>
+        <v>463.9618914487116</v>
       </c>
       <c r="H10" t="n">
-        <v>75659.45807402786</v>
+        <v>3895.392651554141</v>
       </c>
       <c r="I10" t="n">
-        <v>51.91781151231434</v>
+        <v>118.0287782037461</v>
       </c>
       <c r="J10" t="n">
-        <v>0.3244184923225048</v>
+        <v>0.7375256614282456</v>
       </c>
       <c r="K10" t="n">
-        <v>223451.2939094523</v>
+        <v>115.7461975536342</v>
       </c>
       <c r="L10" t="n">
-        <v>241607.8345365945</v>
+        <v>2165.622104179397</v>
       </c>
       <c r="M10" t="n">
-        <v>220737.3007720875</v>
+        <v>2049.875906625763</v>
       </c>
       <c r="N10" t="n">
-        <v>238673.3158171298</v>
+        <v>894.9726255294235</v>
       </c>
       <c r="O10" t="n">
-        <v>34720.66816265808</v>
+        <v>847.1389438729115</v>
       </c>
       <c r="P10" t="n">
-        <v>37541.89694619906</v>
+        <v>1972.040338751561</v>
       </c>
       <c r="Q10" t="n">
-        <v>260.6741948432603</v>
+        <v>1866.640523062403</v>
       </c>
       <c r="R10" t="n">
-        <v>301.455409737188</v>
+        <v>0.9434057945951708</v>
       </c>
       <c r="S10" t="n">
-        <v>-2.91038304567337e-11</v>
+        <v>0.9526397011065801</v>
       </c>
       <c r="T10" t="n">
-        <v>0</v>
+        <v>49.51571860632898</v>
       </c>
       <c r="U10" t="n">
+        <v>50.89181703795853</v>
+      </c>
+      <c r="V10" t="n">
+        <v>49.52495251284039</v>
+      </c>
+      <c r="W10" t="n">
+        <v>50.9015945285745</v>
+      </c>
+      <c r="X10" t="n">
+        <v>49.52033555958468</v>
+      </c>
+      <c r="Y10" t="n">
+        <v>50.89670578326651</v>
+      </c>
+      <c r="Z10" t="n">
+        <v>2.273736754432321e-13</v>
+      </c>
+      <c r="AA10" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB10" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC10" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1130,63 +1386,87 @@
         <v>9</v>
       </c>
       <c r="B11" t="n">
-        <v>3.093086941691099</v>
+        <v>2047.75658883891</v>
       </c>
       <c r="C11" t="n">
-        <v>0.05398455118295154</v>
+        <v>3.427912938590898</v>
       </c>
       <c r="D11" t="n">
-        <v>62371.03486510162</v>
+        <v>2.932944702391893</v>
       </c>
       <c r="E11" t="n">
-        <v>12.3680178772166</v>
+        <v>50.19454407086326</v>
       </c>
       <c r="F11" t="n">
-        <v>12.34999999999999</v>
+        <v>51.96939412734315</v>
       </c>
       <c r="G11" t="n">
-        <v>3823.103391604091</v>
+        <v>442.5223541413023</v>
       </c>
       <c r="H11" t="n">
-        <v>108518.5126056569</v>
+        <v>4135.007484862293</v>
       </c>
       <c r="I11" t="n">
-        <v>103.8356230246287</v>
+        <v>118.0287782037461</v>
       </c>
       <c r="J11" t="n">
-        <v>0.2760519005232043</v>
+        <v>0.7375256614282456</v>
       </c>
       <c r="K11" t="n">
-        <v>241607.8345365945</v>
+        <v>227.1054545556164</v>
       </c>
       <c r="L11" t="n">
-        <v>254320.3536140678</v>
+        <v>2049.875906625763</v>
       </c>
       <c r="M11" t="n">
-        <v>238673.3158171298</v>
+        <v>1822.770452070146</v>
       </c>
       <c r="N11" t="n">
-        <v>251231.4312707474</v>
+        <v>847.1389438729115</v>
       </c>
       <c r="O11" t="n">
-        <v>37541.89694619906</v>
+        <v>753.2845430781289</v>
       </c>
       <c r="P11" t="n">
-        <v>39517.21402169235</v>
+        <v>1866.640523062403</v>
       </c>
       <c r="Q11" t="n">
-        <v>301.455409737188</v>
+        <v>1659.835690090914</v>
       </c>
       <c r="R11" t="n">
-        <v>362.9397996433237</v>
+        <v>0.6972729670952765</v>
       </c>
       <c r="S11" t="n">
-        <v>2.91038304567337e-11</v>
+        <v>0.7070504577112411</v>
       </c>
       <c r="T11" t="n">
-        <v>0</v>
+        <v>50.89181703795853</v>
       </c>
       <c r="U11" t="n">
+        <v>52.2820774005333</v>
+      </c>
+      <c r="V11" t="n">
+        <v>50.9015945285745</v>
+      </c>
+      <c r="W11" t="n">
+        <v>52.29313173610078</v>
+      </c>
+      <c r="X11" t="n">
+        <v>50.89670578326651</v>
+      </c>
+      <c r="Y11" t="n">
+        <v>52.28760456831704</v>
+      </c>
+      <c r="Z11" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA11" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB11" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC11" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1195,64 +1475,88 @@
         <v>10</v>
       </c>
       <c r="B12" t="n">
-        <v>9.025556359556186</v>
+        <v>2337.296317582523</v>
       </c>
       <c r="C12" t="n">
-        <v>0.1575256752985686</v>
+        <v>3.703398138537016</v>
       </c>
       <c r="D12" t="n">
-        <v>71242.4489983699</v>
+        <v>3.087500000000006</v>
       </c>
       <c r="E12" t="n">
-        <v>12.50482896617596</v>
+        <v>51.96939412734315</v>
       </c>
       <c r="F12" t="n">
-        <v>12.34999999999999</v>
+        <v>54.01517752872294</v>
       </c>
       <c r="G12" t="n">
-        <v>3972.491073373149</v>
+        <v>410.256822054316</v>
       </c>
       <c r="H12" t="n">
-        <v>122436.3747918735</v>
+        <v>4588.837380947503</v>
       </c>
       <c r="I12" t="n">
-        <v>103.8356230246287</v>
+        <v>236.0575564074921</v>
       </c>
       <c r="J12" t="n">
-        <v>0.2760519005232043</v>
+        <v>0.6275701457841255</v>
       </c>
       <c r="K12" t="n">
-        <v>254320.3536140678</v>
+        <v>195.5136001732768</v>
       </c>
       <c r="L12" t="n">
-        <v>256078.2094044912</v>
+        <v>1822.770452070146</v>
       </c>
       <c r="M12" t="n">
-        <v>251231.4312707474</v>
+        <v>1627.256851896869</v>
       </c>
       <c r="N12" t="n">
-        <v>252967.9365088056</v>
+        <v>753.2845430781289</v>
       </c>
       <c r="O12" t="n">
-        <v>39517.21402169235</v>
+        <v>672.4859034003669</v>
       </c>
       <c r="P12" t="n">
-        <v>39790.35599598689</v>
+        <v>1659.835690090914</v>
       </c>
       <c r="Q12" t="n">
-        <v>362.9397996433237</v>
+        <v>1481.798762239024</v>
       </c>
       <c r="R12" t="n">
-        <v>438.6942614259252</v>
+        <v>0.312683273190154</v>
       </c>
       <c r="S12" t="n">
-        <v>2.91038304567337e-11</v>
+        <v>0.32373760875763</v>
       </c>
       <c r="T12" t="n">
-        <v>0</v>
+        <v>52.2820774005333</v>
       </c>
       <c r="U12" t="n">
-        <v>0</v>
+        <v>53.68208561152324</v>
+      </c>
+      <c r="V12" t="n">
+        <v>52.29313173610078</v>
+      </c>
+      <c r="W12" t="n">
+        <v>53.69454824356629</v>
+      </c>
+      <c r="X12" t="n">
+        <v>52.28760456831704</v>
+      </c>
+      <c r="Y12" t="n">
+        <v>53.68831692754476</v>
+      </c>
+      <c r="Z12" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA12" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB12" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC12" t="n">
+        <v>-9.094947017729282e-13</v>
       </c>
     </row>
     <row r="13">
@@ -1260,64 +1564,88 @@
         <v>11</v>
       </c>
       <c r="B13" t="n">
-        <v>14.4626516468614</v>
+        <v>2552.62214290462</v>
       </c>
       <c r="C13" t="n">
-        <v>0.2524208898067117</v>
+        <v>3.816120934206944</v>
       </c>
       <c r="D13" t="n">
-        <v>58104.17109555474</v>
+        <v>3.087500000000006</v>
       </c>
       <c r="E13" t="n">
-        <v>10.26501851563292</v>
+        <v>54.01517752872294</v>
       </c>
       <c r="F13" t="n">
-        <v>9.939726703072068</v>
+        <v>56.25879568493919</v>
       </c>
       <c r="G13" t="n">
-        <v>4036.545955867396</v>
+        <v>365.4864868948921</v>
       </c>
       <c r="H13" t="n">
-        <v>101962.1203276141</v>
+        <v>4798.488515938431</v>
       </c>
       <c r="I13" t="n">
-        <v>103.8356230246287</v>
+        <v>236.0575564074921</v>
       </c>
       <c r="J13" t="n">
-        <v>0.2760519005232043</v>
+        <v>0.6275701457841255</v>
       </c>
       <c r="K13" t="n">
-        <v>256078.2094044912</v>
+        <v>323.9726309030392</v>
       </c>
       <c r="L13" t="n">
-        <v>247679.9309536193</v>
+        <v>1627.256851896869</v>
       </c>
       <c r="M13" t="n">
-        <v>252967.9365088056</v>
+        <v>1303.28422099383</v>
       </c>
       <c r="N13" t="n">
-        <v>244671.6618086507</v>
+        <v>672.4859034003669</v>
       </c>
       <c r="O13" t="n">
-        <v>39790.35599598689</v>
+        <v>538.5998318094809</v>
       </c>
       <c r="P13" t="n">
-        <v>38485.40119295726</v>
+        <v>1481.798762239024</v>
       </c>
       <c r="Q13" t="n">
-        <v>438.6942614259252</v>
+        <v>1186.785566927022</v>
       </c>
       <c r="R13" t="n">
-        <v>517.8327630668458</v>
+        <v>-0.3330919171996999</v>
       </c>
       <c r="S13" t="n">
-        <v>-2.91038304567337e-11</v>
+        <v>-0.3206292851566545</v>
       </c>
       <c r="T13" t="n">
-        <v>0</v>
+        <v>53.68208561152324</v>
       </c>
       <c r="U13" t="n">
-        <v>0</v>
+        <v>54.89568056230333</v>
+      </c>
+      <c r="V13" t="n">
+        <v>53.69454824356629</v>
+      </c>
+      <c r="W13" t="n">
+        <v>54.91144616847353</v>
+      </c>
+      <c r="X13" t="n">
+        <v>53.68831692754476</v>
+      </c>
+      <c r="Y13" t="n">
+        <v>54.90356336538844</v>
+      </c>
+      <c r="Z13" t="n">
+        <v>2.273736754432321e-13</v>
+      </c>
+      <c r="AA13" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB13" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC13" t="n">
+        <v>9.094947017729282e-13</v>
       </c>
     </row>
     <row r="14">
@@ -1325,64 +1653,88 @@
         <v>12</v>
       </c>
       <c r="B14" t="n">
-        <v>19.42544105333852</v>
+        <v>2850.434752540939</v>
       </c>
       <c r="C14" t="n">
-        <v>0.3390379050328326</v>
+        <v>3.947910380595018</v>
       </c>
       <c r="D14" t="n">
-        <v>53281.20743256763</v>
+        <v>3.087499999999977</v>
       </c>
       <c r="E14" t="n">
-        <v>10.53969822999045</v>
+        <v>56.25879568493919</v>
       </c>
       <c r="F14" t="n">
-        <v>9.939726703072068</v>
+        <v>58.72018573139036</v>
       </c>
       <c r="G14" t="n">
-        <v>4007.394400845123</v>
+        <v>277.3545174776504</v>
       </c>
       <c r="H14" t="n">
-        <v>97988.89922008957</v>
+        <v>4931.352135023512</v>
       </c>
       <c r="I14" t="n">
-        <v>103.8356230246287</v>
+        <v>236.0575564074921</v>
       </c>
       <c r="J14" t="n">
-        <v>0.2760519005232043</v>
+        <v>0.6275701457841255</v>
       </c>
       <c r="K14" t="n">
-        <v>247679.9309536193</v>
+        <v>363.4699549730709</v>
       </c>
       <c r="L14" t="n">
-        <v>230608.4400432078</v>
+        <v>1303.28422099383</v>
       </c>
       <c r="M14" t="n">
-        <v>244671.6618086507</v>
+        <v>939.814266020759</v>
       </c>
       <c r="N14" t="n">
-        <v>227807.5176912017</v>
+        <v>538.5998318094809</v>
       </c>
       <c r="O14" t="n">
-        <v>38485.40119295726</v>
+        <v>388.3909568282327</v>
       </c>
       <c r="P14" t="n">
-        <v>35832.77134878899</v>
+        <v>1186.785566927022</v>
       </c>
       <c r="Q14" t="n">
-        <v>517.8327630668458</v>
+        <v>855.8056550819163</v>
       </c>
       <c r="R14" t="n">
-        <v>621.6978971345503</v>
+        <v>-1.363115122635851</v>
       </c>
       <c r="S14" t="n">
-        <v>0</v>
+        <v>-1.347349516465657</v>
       </c>
       <c r="T14" t="n">
-        <v>0</v>
+        <v>54.89568056230333</v>
       </c>
       <c r="U14" t="n">
-        <v>3.725290298461914e-09</v>
+        <v>55.56449066105351</v>
+      </c>
+      <c r="V14" t="n">
+        <v>54.91144616847353</v>
+      </c>
+      <c r="W14" t="n">
+        <v>55.58675438115107</v>
+      </c>
+      <c r="X14" t="n">
+        <v>54.90356336538844</v>
+      </c>
+      <c r="Y14" t="n">
+        <v>55.57562252110229</v>
+      </c>
+      <c r="Z14" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA14" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB14" t="n">
+        <v>9.094947017729282e-13</v>
+      </c>
+      <c r="AC14" t="n">
+        <v>-9.094947017729282e-13</v>
       </c>
     </row>
     <row r="15">
@@ -1390,63 +1742,87 @@
         <v>13</v>
       </c>
       <c r="B15" t="n">
-        <v>24.54520018318539</v>
+        <v>3135.192005918565</v>
       </c>
       <c r="C15" t="n">
-        <v>0.4283945587577004</v>
+        <v>4.10346873060611</v>
       </c>
       <c r="D15" t="n">
-        <v>48538.51240245362</v>
+        <v>3.087500000000006</v>
       </c>
       <c r="E15" t="n">
-        <v>10.92717340841417</v>
+        <v>58.72018573139036</v>
       </c>
       <c r="F15" t="n">
-        <v>9.939726703072068</v>
+        <v>61.42443913628225</v>
       </c>
       <c r="G15" t="n">
-        <v>3889.894774972113</v>
+        <v>174.2044735818435</v>
       </c>
       <c r="H15" t="n">
-        <v>92723.7348333438</v>
+        <v>4979.160624392201</v>
       </c>
       <c r="I15" t="n">
-        <v>103.8356230246287</v>
+        <v>236.0575564074921</v>
       </c>
       <c r="J15" t="n">
-        <v>0.2760519005232043</v>
+        <v>0.6275701457841255</v>
       </c>
       <c r="K15" t="n">
-        <v>230608.4400432078</v>
+        <v>358.8253933957828</v>
       </c>
       <c r="L15" t="n">
-        <v>205705.6884024436</v>
+        <v>939.814266020759</v>
       </c>
       <c r="M15" t="n">
-        <v>227807.5176912017</v>
+        <v>580.9888726249765</v>
       </c>
       <c r="N15" t="n">
-        <v>203207.2297143173</v>
+        <v>388.3909568282327</v>
       </c>
       <c r="O15" t="n">
-        <v>35832.77134878899</v>
+        <v>240.1015097385068</v>
       </c>
       <c r="P15" t="n">
-        <v>31963.29196055847</v>
+        <v>855.8056550819163</v>
       </c>
       <c r="Q15" t="n">
-        <v>621.6978971345503</v>
+        <v>529.0551343058027</v>
       </c>
       <c r="R15" t="n">
-        <v>763.9777224223332</v>
+        <v>-3.155695070336846</v>
       </c>
       <c r="S15" t="n">
-        <v>0</v>
+        <v>-3.133431350239291</v>
       </c>
       <c r="T15" t="n">
-        <v>0</v>
+        <v>55.56449066105351</v>
       </c>
       <c r="U15" t="n">
+        <v>54.61389971343809</v>
+      </c>
+      <c r="V15" t="n">
+        <v>55.58675438115107</v>
+      </c>
+      <c r="W15" t="n">
+        <v>54.6507346784532</v>
+      </c>
+      <c r="X15" t="n">
+        <v>55.57562252110229</v>
+      </c>
+      <c r="Y15" t="n">
+        <v>54.63231719594565</v>
+      </c>
+      <c r="Z15" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA15" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB15" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC15" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1455,63 +1831,87 @@
         <v>14</v>
       </c>
       <c r="B16" t="n">
-        <v>29.8837617113602</v>
+        <v>3410.027598793884</v>
       </c>
       <c r="C16" t="n">
-        <v>0.5215700347446509</v>
+        <v>4.289383295124071</v>
       </c>
       <c r="D16" t="n">
-        <v>43474.14387046653</v>
+        <v>3.087500000000006</v>
       </c>
       <c r="E16" t="n">
-        <v>11.46400365670253</v>
+        <v>61.42443913628225</v>
       </c>
       <c r="F16" t="n">
-        <v>9.939726703072068</v>
+        <v>64.40379640476834</v>
       </c>
       <c r="G16" t="n">
-        <v>3703.845412949474</v>
+        <v>54.95969632550521</v>
       </c>
       <c r="H16" t="n">
-        <v>86017.22004816629</v>
+        <v>4931.406634432699</v>
       </c>
       <c r="I16" t="n">
-        <v>103.8356230246287</v>
+        <v>236.0575564074921</v>
       </c>
       <c r="J16" t="n">
-        <v>0.2760519005232043</v>
+        <v>0.6275701457841255</v>
       </c>
       <c r="K16" t="n">
-        <v>205705.6884024436</v>
+        <v>287.2812881774322</v>
       </c>
       <c r="L16" t="n">
-        <v>173940.9557781213</v>
+        <v>580.9888726249765</v>
       </c>
       <c r="M16" t="n">
-        <v>203207.2297143173</v>
+        <v>293.7075844475443</v>
       </c>
       <c r="N16" t="n">
-        <v>171828.3049537327</v>
+        <v>240.1015097385068</v>
       </c>
       <c r="O16" t="n">
-        <v>31963.29196055847</v>
+        <v>121.378631795286</v>
       </c>
       <c r="P16" t="n">
-        <v>27027.57321206211</v>
+        <v>529.0551343058027</v>
       </c>
       <c r="Q16" t="n">
-        <v>763.9777224223332</v>
+        <v>267.4534967158136</v>
       </c>
       <c r="R16" t="n">
-        <v>972.4557268311504</v>
+        <v>-6.81053942284416</v>
       </c>
       <c r="S16" t="n">
-        <v>2.91038304567337e-11</v>
+        <v>-6.773704457829049</v>
       </c>
       <c r="T16" t="n">
-        <v>-3.637978807091713e-12</v>
+        <v>54.61389971343809</v>
       </c>
       <c r="U16" t="n">
+        <v>48.58090923672728</v>
+      </c>
+      <c r="V16" t="n">
+        <v>54.6507346784532</v>
+      </c>
+      <c r="W16" t="n">
+        <v>48.65548365701611</v>
+      </c>
+      <c r="X16" t="n">
+        <v>54.63231719594565</v>
+      </c>
+      <c r="Y16" t="n">
+        <v>48.61819644687169</v>
+      </c>
+      <c r="Z16" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA16" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB16" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC16" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1520,64 +1920,88 @@
         <v>15</v>
       </c>
       <c r="B17" t="n">
-        <v>35.52605335902853</v>
+        <v>3337.28873555677</v>
       </c>
       <c r="C17" t="n">
-        <v>0.6200466013542391</v>
+        <v>4.515209574421058</v>
       </c>
       <c r="D17" t="n">
-        <v>38503.67616132362</v>
+        <v>3.087499999999977</v>
       </c>
       <c r="E17" t="n">
-        <v>12.21319636798589</v>
+        <v>64.40379640476834</v>
       </c>
       <c r="F17" t="n">
-        <v>9.93972670307204</v>
+        <v>67.70078395860372</v>
       </c>
       <c r="G17" t="n">
-        <v>3382.563080247126</v>
+        <v>0</v>
       </c>
       <c r="H17" t="n">
-        <v>77643.23955338272</v>
+        <v>4712.381334936381</v>
       </c>
       <c r="I17" t="n">
-        <v>103.8356230246287</v>
+        <v>236.0575564074921</v>
       </c>
       <c r="J17" t="n">
-        <v>0.2760519005232043</v>
+        <v>0.6275701457841255</v>
       </c>
       <c r="K17" t="n">
-        <v>173940.9557781213</v>
+        <v>301.0630465167167</v>
       </c>
       <c r="L17" t="n">
-        <v>136793.6190736684</v>
+        <v>293.7075844475443</v>
       </c>
       <c r="M17" t="n">
-        <v>171828.3049537327</v>
+        <v>-7.355462069172778</v>
       </c>
       <c r="N17" t="n">
-        <v>135132.1521073967</v>
+        <v>121.378631795286</v>
       </c>
       <c r="O17" t="n">
-        <v>27027.57321206211</v>
+        <v>-3.039744185897137</v>
       </c>
       <c r="P17" t="n">
-        <v>21255.48602350242</v>
+        <v>267.4534967158136</v>
       </c>
       <c r="Q17" t="n">
-        <v>972.4557268311504</v>
+        <v>-6.697968164700698</v>
       </c>
       <c r="R17" t="n">
-        <v>1308.305528633337</v>
+        <v>-15.82288716804106</v>
       </c>
       <c r="S17" t="n">
-        <v>-2.91038304567337e-11</v>
+        <v>-15.74831274775223</v>
       </c>
       <c r="T17" t="n">
-        <v>0</v>
+        <v>48.58090923672728</v>
       </c>
       <c r="U17" t="n">
-        <v>-3.725290298461914e-09</v>
+        <v>736.4678451674736</v>
+      </c>
+      <c r="V17" t="n">
+        <v>48.65548365701611</v>
+      </c>
+      <c r="W17" t="n">
+        <v>733.3927721120749</v>
+      </c>
+      <c r="X17" t="n">
+        <v>48.61819644687169</v>
+      </c>
+      <c r="Y17" t="n">
+        <v>734.9303086397742</v>
+      </c>
+      <c r="Z17" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA17" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB17" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC17" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="18">
@@ -1585,63 +2009,87 @@
         <v>16</v>
       </c>
       <c r="B18" t="n">
-        <v>41.59830918914744</v>
+        <v>2938.964788325616</v>
       </c>
       <c r="C18" t="n">
-        <v>0.7260274586132355</v>
+        <v>4.795427561821701</v>
       </c>
       <c r="D18" t="n">
-        <v>33106.37001493151</v>
+        <v>3.087500000000006</v>
       </c>
       <c r="E18" t="n">
-        <v>13.291644383338</v>
+        <v>67.70078395860372</v>
       </c>
       <c r="F18" t="n">
-        <v>9.939726703072068</v>
+        <v>71.37341370684827</v>
       </c>
       <c r="G18" t="n">
-        <v>2938.392420201765</v>
+        <v>0</v>
       </c>
       <c r="H18" t="n">
-        <v>67246.54663088753</v>
+        <v>4320.51990554777</v>
       </c>
       <c r="I18" t="n">
-        <v>103.8356230246287</v>
+        <v>236.0575564074921</v>
       </c>
       <c r="J18" t="n">
-        <v>0.2760519005232043</v>
+        <v>0.6275701457841255</v>
       </c>
       <c r="K18" t="n">
-        <v>136793.6190736684</v>
+        <v>365.0707135084249</v>
       </c>
       <c r="L18" t="n">
-        <v>96258.81121913623</v>
+        <v>-7.355462069172778</v>
       </c>
       <c r="M18" t="n">
-        <v>135132.1521073967</v>
+        <v>-372.426175577598</v>
       </c>
       <c r="N18" t="n">
-        <v>95089.6716339992</v>
+        <v>-3.039744185897137</v>
       </c>
       <c r="O18" t="n">
-        <v>21255.48602350242</v>
+        <v>-153.9101542828332</v>
       </c>
       <c r="P18" t="n">
-        <v>14957.04134712195</v>
+        <v>-6.697968164700698</v>
       </c>
       <c r="Q18" t="n">
-        <v>1308.305528633337</v>
+        <v>-339.1355491009315</v>
       </c>
       <c r="R18" t="n">
-        <v>1935.73315811179</v>
+        <v>668.7670612088699</v>
       </c>
       <c r="S18" t="n">
-        <v>0</v>
+        <v>665.6919881534711</v>
       </c>
       <c r="T18" t="n">
-        <v>5.456968210637569e-12</v>
+        <v>736.4678451674736</v>
       </c>
       <c r="U18" t="n">
+        <v>83.4251516595978</v>
+      </c>
+      <c r="V18" t="n">
+        <v>733.3927721120749</v>
+      </c>
+      <c r="W18" t="n">
+        <v>83.36111543953196</v>
+      </c>
+      <c r="X18" t="n">
+        <v>734.9303086397742</v>
+      </c>
+      <c r="Y18" t="n">
+        <v>83.39313354956488</v>
+      </c>
+      <c r="Z18" t="n">
+        <v>1.13686837721616e-13</v>
+      </c>
+      <c r="AA18" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB18" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC18" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1650,64 +2098,88 @@
         <v>17</v>
       </c>
       <c r="B19" t="n">
-        <v>48.30835694146017</v>
+        <v>2410.279926466423</v>
       </c>
       <c r="C19" t="n">
-        <v>0.8431398848571375</v>
+        <v>5.153245914347297</v>
       </c>
       <c r="D19" t="n">
-        <v>26610.08740263997</v>
+        <v>3.087500000000006</v>
       </c>
       <c r="E19" t="n">
-        <v>14.94422825432905</v>
+        <v>71.37341370684827</v>
       </c>
       <c r="F19" t="n">
-        <v>9.939726703072068</v>
+        <v>75.50440019361704</v>
       </c>
       <c r="G19" t="n">
-        <v>2369.452663956918</v>
+        <v>0</v>
       </c>
       <c r="H19" t="n">
-        <v>54248.53262366771</v>
+        <v>3762.856786028168</v>
       </c>
       <c r="I19" t="n">
-        <v>103.8356230246287</v>
+        <v>236.0575564074921</v>
       </c>
       <c r="J19" t="n">
-        <v>0.2760519005232043</v>
+        <v>0.6275701457841255</v>
       </c>
       <c r="K19" t="n">
-        <v>96258.81121913623</v>
+        <v>323.6158265055616</v>
       </c>
       <c r="L19" t="n">
-        <v>55367.76596963337</v>
+        <v>-372.426175577598</v>
       </c>
       <c r="M19" t="n">
-        <v>95089.6716339992</v>
+        <v>-696.0420020831596</v>
       </c>
       <c r="N19" t="n">
-        <v>54695.28055125089</v>
+        <v>-153.9101542828332</v>
       </c>
       <c r="O19" t="n">
-        <v>14957.04134712195</v>
+        <v>-287.6487716305275</v>
       </c>
       <c r="P19" t="n">
-        <v>8603.243219161472</v>
+        <v>-339.1355491009315</v>
       </c>
       <c r="Q19" t="n">
-        <v>1935.73315811179</v>
+        <v>-633.8238342342308</v>
       </c>
       <c r="R19" t="n">
-        <v>3451.867030936333</v>
+        <v>12.05173795274953</v>
       </c>
       <c r="S19" t="n">
-        <v>-1.455191522836685e-11</v>
+        <v>11.98770173268369</v>
       </c>
       <c r="T19" t="n">
+        <v>83.4251516595978</v>
+      </c>
+      <c r="U19" t="n">
+        <v>79.85881765422408</v>
+      </c>
+      <c r="V19" t="n">
+        <v>83.36111543953196</v>
+      </c>
+      <c r="W19" t="n">
+        <v>79.82220267794803</v>
+      </c>
+      <c r="X19" t="n">
+        <v>83.39313354956488</v>
+      </c>
+      <c r="Y19" t="n">
+        <v>79.84051016608606</v>
+      </c>
+      <c r="Z19" t="n">
+        <v>-1.13686837721616e-13</v>
+      </c>
+      <c r="AA19" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB19" t="n">
         <v>-1.818989403545856e-12</v>
       </c>
-      <c r="U19" t="n">
-        <v>0</v>
+      <c r="AC19" t="n">
+        <v>-9.094947017729282e-13</v>
       </c>
     </row>
     <row r="20">
@@ -1715,64 +2187,88 @@
         <v>18</v>
       </c>
       <c r="B20" t="n">
-        <v>56.05420832385308</v>
+        <v>1226.217337404106</v>
       </c>
       <c r="C20" t="n">
-        <v>0.9783304948500482</v>
+        <v>4.753541162170476</v>
       </c>
       <c r="D20" t="n">
-        <v>19840.17967533819</v>
+        <v>2.62652581469689</v>
       </c>
       <c r="E20" t="n">
-        <v>17.80010592668061</v>
+        <v>75.50440019361704</v>
       </c>
       <c r="F20" t="n">
-        <v>9.939726703072068</v>
+        <v>79.47126890591167</v>
       </c>
       <c r="G20" t="n">
-        <v>1620.674247115495</v>
+        <v>0</v>
       </c>
       <c r="H20" t="n">
-        <v>38974.45926823906</v>
+        <v>2243.677253601692</v>
       </c>
       <c r="I20" t="n">
-        <v>103.8356230246287</v>
+        <v>236.0575564074921</v>
       </c>
       <c r="J20" t="n">
-        <v>0.2760519005232043</v>
+        <v>0.6275701457841255</v>
       </c>
       <c r="K20" t="n">
-        <v>55367.76596963337</v>
+        <v>-25.45256421161733</v>
       </c>
       <c r="L20" t="n">
-        <v>18621.69573402152</v>
+        <v>-696.0420020831596</v>
       </c>
       <c r="M20" t="n">
-        <v>54695.28055125089</v>
+        <v>-670.5894378715421</v>
       </c>
       <c r="N20" t="n">
-        <v>18395.52047433066</v>
+        <v>-287.6487716305275</v>
       </c>
       <c r="O20" t="n">
-        <v>8603.243219161472</v>
+        <v>-277.1301552131175</v>
       </c>
       <c r="P20" t="n">
-        <v>2893.506262125056</v>
+        <v>-633.8238342342308</v>
       </c>
       <c r="Q20" t="n">
-        <v>3451.867030936333</v>
+        <v>-610.6464371929344</v>
       </c>
       <c r="R20" t="n">
-        <v>10388.95381502454</v>
+        <v>4.354417460607042</v>
       </c>
       <c r="S20" t="n">
-        <v>0</v>
+        <v>4.317802484330987</v>
       </c>
       <c r="T20" t="n">
-        <v>-1.818989403545856e-12</v>
+        <v>79.85881765422408</v>
       </c>
       <c r="U20" t="n">
-        <v>0</v>
+        <v>81.16333703991899</v>
+      </c>
+      <c r="V20" t="n">
+        <v>79.82220267794803</v>
+      </c>
+      <c r="W20" t="n">
+        <v>81.12551677443921</v>
+      </c>
+      <c r="X20" t="n">
+        <v>79.84051016608606</v>
+      </c>
+      <c r="Y20" t="n">
+        <v>81.1444269071791</v>
+      </c>
+      <c r="Z20" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA20" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB20" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC20" t="n">
+        <v>-4.547473508864641e-13</v>
       </c>
     </row>
     <row r="21">
@@ -1780,64 +2276,88 @@
         <v>19</v>
       </c>
       <c r="B21" t="n">
-        <v>65.8387755279059</v>
+        <v>17.10770091220042</v>
       </c>
       <c r="C21" t="n">
-        <v>1.149103408443426</v>
+        <v>5.210866479545521</v>
       </c>
       <c r="D21" t="n">
-        <v>10045.72056946627</v>
+        <v>2.62652581469689</v>
       </c>
       <c r="E21" t="n">
-        <v>24.28436213742816</v>
+        <v>79.47126890591167</v>
       </c>
       <c r="F21" t="n">
-        <v>9.939726703072068</v>
+        <v>83.97975317326198</v>
       </c>
       <c r="G21" t="n">
-        <v>514.3747927753163</v>
+        <v>0</v>
       </c>
       <c r="H21" t="n">
-        <v>16948.91230046818</v>
+        <v>803.1419985264261</v>
       </c>
       <c r="I21" t="n">
-        <v>103.8356230246287</v>
+        <v>236.0575564074921</v>
       </c>
       <c r="J21" t="n">
-        <v>0.2760519005232043</v>
+        <v>0.6275701457841255</v>
       </c>
       <c r="K21" t="n">
-        <v>18621.69573402152</v>
+        <v>-670.590449859892</v>
       </c>
       <c r="L21" t="n">
-        <v>-0.004123225935407311</v>
+        <v>-670.5894378715421</v>
       </c>
       <c r="M21" t="n">
-        <v>18395.52047433066</v>
+        <v>0.001011988349920594</v>
       </c>
       <c r="N21" t="n">
-        <v>-0.004073146087147248</v>
+        <v>-277.1301552131175</v>
       </c>
       <c r="O21" t="n">
-        <v>2893.506262125056</v>
+        <v>0.0004182178731855961</v>
       </c>
       <c r="P21" t="n">
-        <v>-0.0006406817206480573</v>
+        <v>-610.6464371929344</v>
       </c>
       <c r="Q21" t="n">
-        <v>10388.95381502454</v>
+        <v>0.0009215282040844562</v>
       </c>
       <c r="R21" t="n">
-        <v>-47062254395.20467</v>
+        <v>1.692068134007313</v>
       </c>
       <c r="S21" t="n">
-        <v>0</v>
+        <v>1.654247868527539</v>
       </c>
       <c r="T21" t="n">
-        <v>0</v>
+        <v>81.16333703991899</v>
       </c>
       <c r="U21" t="n">
-        <v>0</v>
+        <v>-19686.06366446138</v>
+      </c>
+      <c r="V21" t="n">
+        <v>81.12551677443921</v>
+      </c>
+      <c r="W21" t="n">
+        <v>83.97975317326198</v>
+      </c>
+      <c r="X21" t="n">
+        <v>81.1444269071791</v>
+      </c>
+      <c r="Y21" t="n">
+        <v>-9801.041955644057</v>
+      </c>
+      <c r="Z21" t="n">
+        <v>-1.77635683940025e-15</v>
+      </c>
+      <c r="AA21" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB21" t="n">
+        <v>7.105427357601002e-15</v>
+      </c>
+      <c r="AC21" t="n">
+        <v>-7.105427357601002e-15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Implemented force equilibrium method (COE).
</commit_message>
<xml_diff>
--- a/thrust_calc_resuls.xlsx
+++ b/thrust_calc_resuls.xlsx
@@ -585,52 +585,52 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>82.81710392252958</v>
+        <v>6551.324978560411</v>
       </c>
       <c r="C2" t="n">
-        <v>1.498547206397035</v>
+        <v>7.270885335184865</v>
       </c>
       <c r="D2" t="n">
-        <v>1.466472351195947</v>
+        <v>5.011864557945543</v>
       </c>
       <c r="E2" t="n">
-        <v>40.2112427661442</v>
+        <v>39.99961494556892</v>
       </c>
       <c r="F2" t="n">
-        <v>40.51964175793073</v>
+        <v>34.72697403083298</v>
       </c>
       <c r="G2" t="n">
-        <v>28.1884498624697</v>
+        <v>169.5230309342399</v>
       </c>
       <c r="H2" t="n">
-        <v>79.49535066612499</v>
+        <v>1797.286764508279</v>
       </c>
       <c r="I2" t="n">
-        <v>117.940321739393</v>
+        <v>207.449762184769</v>
       </c>
       <c r="J2" t="n">
-        <v>0.7369729240927206</v>
+        <v>0.264252333311767</v>
       </c>
       <c r="K2" t="n">
-        <v>-226.402310599181</v>
+        <v>-7966.4143526538</v>
       </c>
       <c r="L2" t="n">
         <v>0</v>
       </c>
       <c r="M2" t="n">
-        <v>226.402310599181</v>
+        <v>7966.414352653802</v>
       </c>
       <c r="N2" t="n">
         <v>0</v>
       </c>
       <c r="O2" t="n">
-        <v>91.81820987744683</v>
+        <v>1221.251722124082</v>
       </c>
       <c r="P2" t="n">
         <v>0</v>
       </c>
       <c r="Q2" t="n">
-        <v>206.9478740638549</v>
+        <v>7872.248844477507</v>
       </c>
       <c r="R2" t="n">
         <v>0</v>
@@ -639,25 +639,25 @@
         <v>0</v>
       </c>
       <c r="T2" t="n">
-        <v>40.2112427661442</v>
+        <v>39.99961494556892</v>
       </c>
       <c r="U2" t="n">
-        <v>40.69076896068975</v>
+        <v>37.74949923191704</v>
       </c>
       <c r="V2" t="n">
-        <v>40.2112427661442</v>
+        <v>39.99961494556892</v>
       </c>
       <c r="W2" t="n">
-        <v>40.7013934533427</v>
+        <v>39.15230400500617</v>
       </c>
       <c r="X2" t="n">
-        <v>40.2112427661442</v>
+        <v>39.99961494556892</v>
       </c>
       <c r="Y2" t="n">
-        <v>40.69608120701623</v>
+        <v>38.4509016184616</v>
       </c>
       <c r="Z2" t="n">
-        <v>2.842170943040401e-14</v>
+        <v>2.273736754432321e-13</v>
       </c>
       <c r="AA2" t="n">
         <v>0</v>
@@ -674,85 +674,85 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>148.4582236939683</v>
+        <v>10040.81426160309</v>
       </c>
       <c r="C3" t="n">
-        <v>1.504229717970171</v>
+        <v>6.859044479204075</v>
       </c>
       <c r="D3" t="n">
-        <v>1.466472351195932</v>
+        <v>5.011864557945543</v>
       </c>
       <c r="E3" t="n">
-        <v>40.51964175793073</v>
+        <v>34.72697403083298</v>
       </c>
       <c r="F3" t="n">
-        <v>40.8545666849556</v>
+        <v>30.04068289318306</v>
       </c>
       <c r="G3" t="n">
-        <v>82.31466729253724</v>
+        <v>479.4387895776507</v>
       </c>
       <c r="H3" t="n">
-        <v>232.1388147738423</v>
+        <v>5083.020201744986</v>
       </c>
       <c r="I3" t="n">
-        <v>117.940321739393</v>
+        <v>207.449762184769</v>
       </c>
       <c r="J3" t="n">
-        <v>0.7369729240927206</v>
+        <v>0.264252333311767</v>
       </c>
       <c r="K3" t="n">
-        <v>-239.5849635585784</v>
+        <v>-12222.92797111464</v>
       </c>
       <c r="L3" t="n">
-        <v>226.402310599181</v>
+        <v>7966.414352653802</v>
       </c>
       <c r="M3" t="n">
-        <v>465.9872741577593</v>
+        <v>20189.34232376845</v>
       </c>
       <c r="N3" t="n">
-        <v>91.81820987744683</v>
+        <v>1221.251722124082</v>
       </c>
       <c r="O3" t="n">
-        <v>188.9826884964277</v>
+        <v>3095.027196676161</v>
       </c>
       <c r="P3" t="n">
-        <v>206.9478740638549</v>
+        <v>7872.248844477507</v>
       </c>
       <c r="Q3" t="n">
-        <v>425.945634002323</v>
+        <v>19950.69798573831</v>
       </c>
       <c r="R3" t="n">
-        <v>0.1711272027590224</v>
+        <v>3.022525201084059</v>
       </c>
       <c r="S3" t="n">
-        <v>0.181751695411972</v>
+        <v>4.425329974173189</v>
       </c>
       <c r="T3" t="n">
-        <v>40.69076896068975</v>
+        <v>37.74949923191704</v>
       </c>
       <c r="U3" t="n">
-        <v>41.17226761320322</v>
+        <v>35.04210773626257</v>
       </c>
       <c r="V3" t="n">
-        <v>40.7013934533427</v>
+        <v>39.15230400500617</v>
       </c>
       <c r="W3" t="n">
-        <v>41.177422808244</v>
+        <v>35.59780612380629</v>
       </c>
       <c r="X3" t="n">
-        <v>40.69608120701623</v>
+        <v>38.4509016184616</v>
       </c>
       <c r="Y3" t="n">
-        <v>41.17484521072361</v>
+        <v>35.31995693003443</v>
       </c>
       <c r="Z3" t="n">
-        <v>0</v>
+        <v>1.818989403545856e-12</v>
       </c>
       <c r="AA3" t="n">
-        <v>0</v>
+        <v>1.364242052659392e-12</v>
       </c>
       <c r="AB3" t="n">
-        <v>0</v>
+        <v>-7.275957614183426e-12</v>
       </c>
       <c r="AC3" t="n">
         <v>0</v>
@@ -763,85 +763,85 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>208.161892046477</v>
+        <v>12292.79161631789</v>
       </c>
       <c r="C4" t="n">
-        <v>1.510432428664756</v>
+        <v>6.529337568857022</v>
       </c>
       <c r="D4" t="n">
-        <v>1.466472351195947</v>
+        <v>5.011864557945529</v>
       </c>
       <c r="E4" t="n">
-        <v>40.8545666849556</v>
+        <v>30.04068289318306</v>
       </c>
       <c r="F4" t="n">
-        <v>41.21633377148819</v>
+        <v>25.85314164552767</v>
       </c>
       <c r="G4" t="n">
-        <v>134.7760356084809</v>
+        <v>755.7257942834093</v>
       </c>
       <c r="H4" t="n">
-        <v>380.0871727377647</v>
+        <v>8012.220877468611</v>
       </c>
       <c r="I4" t="n">
-        <v>117.940321739393</v>
+        <v>207.449762184769</v>
       </c>
       <c r="J4" t="n">
-        <v>0.7369729240927206</v>
+        <v>0.264252333311767</v>
       </c>
       <c r="K4" t="n">
-        <v>-244.2808110108978</v>
+        <v>-14749.06899242075</v>
       </c>
       <c r="L4" t="n">
-        <v>465.9872741577593</v>
+        <v>20189.34232376845</v>
       </c>
       <c r="M4" t="n">
-        <v>710.2680851686571</v>
+        <v>34938.4113161892</v>
       </c>
       <c r="N4" t="n">
-        <v>188.9826884964277</v>
+        <v>3095.027196676161</v>
       </c>
       <c r="O4" t="n">
-        <v>288.0515836639344</v>
+        <v>5356.060217224534</v>
       </c>
       <c r="P4" t="n">
-        <v>425.945634002323</v>
+        <v>19950.69798573831</v>
       </c>
       <c r="Q4" t="n">
-        <v>649.2357337345582</v>
+        <v>34525.42837168979</v>
       </c>
       <c r="R4" t="n">
-        <v>0.3177009282476249</v>
+        <v>5.001424843079513</v>
       </c>
       <c r="S4" t="n">
-        <v>0.3228561232883959</v>
+        <v>5.557123230623226</v>
       </c>
       <c r="T4" t="n">
-        <v>41.17226761320322</v>
+        <v>35.04210773626257</v>
       </c>
       <c r="U4" t="n">
-        <v>41.66396949483367</v>
+        <v>32.6597508830049</v>
       </c>
       <c r="V4" t="n">
-        <v>41.177422808244</v>
+        <v>35.59780612380629</v>
       </c>
       <c r="W4" t="n">
-        <v>41.66734670364858</v>
+        <v>32.98197530036523</v>
       </c>
       <c r="X4" t="n">
-        <v>41.17484521072361</v>
+        <v>35.31995693003443</v>
       </c>
       <c r="Y4" t="n">
-        <v>41.66565809924113</v>
+        <v>32.82086309168507</v>
       </c>
       <c r="Z4" t="n">
-        <v>1.13686837721616e-13</v>
+        <v>0</v>
       </c>
       <c r="AA4" t="n">
-        <v>0</v>
+        <v>4.547473508864641e-13</v>
       </c>
       <c r="AB4" t="n">
-        <v>0</v>
+        <v>1.455191522836685e-11</v>
       </c>
       <c r="AC4" t="n">
         <v>0</v>
@@ -852,76 +852,76 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>262.296224566014</v>
+        <v>13804.43695853531</v>
       </c>
       <c r="C5" t="n">
-        <v>1.51717368733887</v>
+        <v>6.259986823385099</v>
       </c>
       <c r="D5" t="n">
-        <v>1.466472351195947</v>
+        <v>5.011864557945543</v>
       </c>
       <c r="E5" t="n">
-        <v>41.21633377148819</v>
+        <v>25.85314164552767</v>
       </c>
       <c r="F5" t="n">
-        <v>41.60529025955755</v>
+        <v>22.10032906584962</v>
       </c>
       <c r="G5" t="n">
-        <v>185.5518678522894</v>
+        <v>1003.035290420923</v>
       </c>
       <c r="H5" t="n">
-        <v>523.282084457974</v>
+        <v>10634.20139360031</v>
       </c>
       <c r="I5" t="n">
-        <v>117.940321739393</v>
+        <v>207.449762184769</v>
       </c>
       <c r="J5" t="n">
-        <v>0.7369729240927206</v>
+        <v>0.264252333311767</v>
       </c>
       <c r="K5" t="n">
-        <v>-241.1090942600918</v>
+        <v>-16185.024744787</v>
       </c>
       <c r="L5" t="n">
-        <v>710.2680851686571</v>
+        <v>34938.4113161892</v>
       </c>
       <c r="M5" t="n">
-        <v>951.3771794287491</v>
+        <v>51123.43606097621</v>
       </c>
       <c r="N5" t="n">
-        <v>288.0515836639344</v>
+        <v>5356.060217224534</v>
       </c>
       <c r="O5" t="n">
-        <v>385.8341785568255</v>
+        <v>7837.225327046808</v>
       </c>
       <c r="P5" t="n">
-        <v>649.2357337345582</v>
+        <v>34525.42837168979</v>
       </c>
       <c r="Q5" t="n">
-        <v>869.6266579372908</v>
+        <v>50519.1410640939</v>
       </c>
       <c r="R5" t="n">
-        <v>0.4476357233454775</v>
+        <v>6.806609237477232</v>
       </c>
       <c r="S5" t="n">
-        <v>0.4510129321603799</v>
+        <v>7.128833654837559</v>
       </c>
       <c r="T5" t="n">
-        <v>41.66396949483367</v>
+        <v>32.6597508830049</v>
       </c>
       <c r="U5" t="n">
-        <v>42.16800826583827</v>
+        <v>30.56493870285103</v>
       </c>
       <c r="V5" t="n">
-        <v>41.66734670364858</v>
+        <v>32.98197530036523</v>
       </c>
       <c r="W5" t="n">
-        <v>42.17052557291126</v>
+        <v>30.78578190796429</v>
       </c>
       <c r="X5" t="n">
-        <v>41.66565809924113</v>
+        <v>32.82086309168507</v>
       </c>
       <c r="Y5" t="n">
-        <v>42.16926691937476</v>
+        <v>30.67536030540766</v>
       </c>
       <c r="Z5" t="n">
         <v>0</v>
@@ -930,10 +930,10 @@
         <v>0</v>
       </c>
       <c r="AB5" t="n">
-        <v>0</v>
+        <v>5.093170329928398e-11</v>
       </c>
       <c r="AC5" t="n">
-        <v>0</v>
+        <v>-2.182787284255028e-11</v>
       </c>
     </row>
     <row r="6">
@@ -941,88 +941,88 @@
         <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>311.1937512784731</v>
+        <v>14838.49774374495</v>
       </c>
       <c r="C6" t="n">
-        <v>1.524473886669827</v>
+        <v>6.036655848649859</v>
       </c>
       <c r="D6" t="n">
-        <v>1.466472351195947</v>
+        <v>5.011864557945543</v>
       </c>
       <c r="E6" t="n">
-        <v>41.60529025955755</v>
+        <v>22.10032906584962</v>
       </c>
       <c r="F6" t="n">
-        <v>42.02181620546986</v>
+        <v>18.73390188558466</v>
       </c>
       <c r="G6" t="n">
-        <v>234.6194871735949</v>
+        <v>1224.826474131253</v>
       </c>
       <c r="H6" t="n">
-        <v>661.6595980612478</v>
+        <v>12985.63622089426</v>
       </c>
       <c r="I6" t="n">
-        <v>117.940321739393</v>
+        <v>207.449762184769</v>
       </c>
       <c r="J6" t="n">
-        <v>0.7369729240927206</v>
+        <v>0.264252333311767</v>
       </c>
       <c r="K6" t="n">
-        <v>-230.6473019482951</v>
+        <v>-16887.27412702405</v>
       </c>
       <c r="L6" t="n">
-        <v>951.3771794287491</v>
+        <v>51123.43606097621</v>
       </c>
       <c r="M6" t="n">
-        <v>1182.024481377044</v>
+        <v>68010.71018800026</v>
       </c>
       <c r="N6" t="n">
-        <v>385.8341785568255</v>
+        <v>7837.225327046808</v>
       </c>
       <c r="O6" t="n">
-        <v>479.3739587909943</v>
+        <v>10426.04530259068</v>
       </c>
       <c r="P6" t="n">
-        <v>869.6266579372908</v>
+        <v>50519.1410640939</v>
       </c>
       <c r="Q6" t="n">
-        <v>1080.454757131329</v>
+        <v>67206.80233149386</v>
       </c>
       <c r="R6" t="n">
-        <v>0.5627180062807261</v>
+        <v>8.464609637001409</v>
       </c>
       <c r="S6" t="n">
-        <v>0.5652353133537118</v>
+        <v>8.685452842114669</v>
       </c>
       <c r="T6" t="n">
-        <v>42.16800826583827</v>
+        <v>30.56493870285103</v>
       </c>
       <c r="U6" t="n">
-        <v>42.68600741569604</v>
+        <v>28.72599071159767</v>
       </c>
       <c r="V6" t="n">
-        <v>42.17052557291126</v>
+        <v>30.78578190796429</v>
       </c>
       <c r="W6" t="n">
-        <v>42.68803015252422</v>
+        <v>28.89238164950081</v>
       </c>
       <c r="X6" t="n">
-        <v>42.16926691937476</v>
+        <v>30.67536030540766</v>
       </c>
       <c r="Y6" t="n">
-        <v>42.68701878411013</v>
+        <v>28.80918618054924</v>
       </c>
       <c r="Z6" t="n">
-        <v>1.13686837721616e-13</v>
+        <v>0</v>
       </c>
       <c r="AA6" t="n">
-        <v>0</v>
+        <v>-2.728484105318785e-12</v>
       </c>
       <c r="AB6" t="n">
-        <v>-5.684341886080801e-14</v>
+        <v>-2.91038304567337e-11</v>
       </c>
       <c r="AC6" t="n">
-        <v>-5.684341886080801e-14</v>
+        <v>-2.91038304567337e-11</v>
       </c>
     </row>
     <row r="7">
@@ -1030,88 +1030,88 @@
         <v>5</v>
       </c>
       <c r="B7" t="n">
-        <v>355.1551194345751</v>
+        <v>15546.37313160678</v>
       </c>
       <c r="C7" t="n">
-        <v>1.532355647855679</v>
+        <v>5.849489621526452</v>
       </c>
       <c r="D7" t="n">
-        <v>1.466472351195932</v>
+        <v>5.011864557945543</v>
       </c>
       <c r="E7" t="n">
-        <v>42.02181620546986</v>
+        <v>18.73390188558466</v>
       </c>
       <c r="F7" t="n">
-        <v>42.46632650231609</v>
+        <v>15.71643411866143</v>
       </c>
       <c r="G7" t="n">
-        <v>281.9541078708978</v>
+        <v>1423.746381713643</v>
       </c>
       <c r="H7" t="n">
-        <v>795.1498144207443</v>
+        <v>15094.58929425999</v>
       </c>
       <c r="I7" t="n">
-        <v>117.940321739393</v>
+        <v>207.449762184769</v>
       </c>
       <c r="J7" t="n">
-        <v>0.7369729240927206</v>
+        <v>0.264252333311767</v>
       </c>
       <c r="K7" t="n">
-        <v>-213.4364949768804</v>
+        <v>-17072.14283421301</v>
       </c>
       <c r="L7" t="n">
-        <v>1182.024481377044</v>
+        <v>68010.71018800026</v>
       </c>
       <c r="M7" t="n">
-        <v>1395.460976353924</v>
+        <v>85082.85302221328</v>
       </c>
       <c r="N7" t="n">
-        <v>479.3739587909943</v>
+        <v>10426.04530259068</v>
       </c>
       <c r="O7" t="n">
-        <v>565.933839029976</v>
+        <v>13043.20566027224</v>
       </c>
       <c r="P7" t="n">
-        <v>1080.454757131329</v>
+        <v>67206.80233149386</v>
       </c>
       <c r="Q7" t="n">
-        <v>1275.550950126039</v>
+        <v>84077.1471001686</v>
       </c>
       <c r="R7" t="n">
-        <v>0.6641912102261809</v>
+        <v>9.992088826013012</v>
       </c>
       <c r="S7" t="n">
-        <v>0.6662139470543561</v>
+        <v>10.15847976391615</v>
       </c>
       <c r="T7" t="n">
-        <v>42.68600741569604</v>
+        <v>28.72599071159767</v>
       </c>
       <c r="U7" t="n">
-        <v>43.21929797879984</v>
+        <v>27.11769645340559</v>
       </c>
       <c r="V7" t="n">
-        <v>42.68803015252422</v>
+        <v>28.89238164950081</v>
       </c>
       <c r="W7" t="n">
-        <v>43.22100845872372</v>
+        <v>27.25094559125544</v>
       </c>
       <c r="X7" t="n">
-        <v>42.68701878411013</v>
+        <v>28.80918618054924</v>
       </c>
       <c r="Y7" t="n">
-        <v>43.22015321876178</v>
+        <v>27.18432102233051</v>
       </c>
       <c r="Z7" t="n">
         <v>0</v>
       </c>
       <c r="AA7" t="n">
-        <v>0</v>
+        <v>1.818989403545856e-12</v>
       </c>
       <c r="AB7" t="n">
-        <v>0</v>
+        <v>-4.365574568510056e-11</v>
       </c>
       <c r="AC7" t="n">
-        <v>0</v>
+        <v>1.01863406598568e-10</v>
       </c>
     </row>
     <row r="8">
@@ -1119,88 +1119,88 @@
         <v>6</v>
       </c>
       <c r="B8" t="n">
-        <v>394.4523145057859</v>
+        <v>16021.12151806232</v>
       </c>
       <c r="C8" t="n">
-        <v>1.540844032415425</v>
+        <v>5.691478441001743</v>
       </c>
       <c r="D8" t="n">
-        <v>1.466472351195947</v>
+        <v>5.011864557945543</v>
       </c>
       <c r="E8" t="n">
-        <v>42.46632650231609</v>
+        <v>15.71643411866143</v>
       </c>
       <c r="F8" t="n">
-        <v>42.93927315549512</v>
+        <v>13.01839398362824</v>
       </c>
       <c r="G8" t="n">
-        <v>327.5287015204694</v>
+        <v>1601.865240390473</v>
       </c>
       <c r="H8" t="n">
-        <v>923.6765096209197</v>
+        <v>16983.00920655716</v>
       </c>
       <c r="I8" t="n">
-        <v>117.940321739393</v>
+        <v>207.449762184769</v>
       </c>
       <c r="J8" t="n">
-        <v>0.7369729240927206</v>
+        <v>0.264252333311767</v>
       </c>
       <c r="K8" t="n">
-        <v>-189.9860839458431</v>
+        <v>-16879.6918536271</v>
       </c>
       <c r="L8" t="n">
-        <v>1395.460976353924</v>
+        <v>85082.85302221328</v>
       </c>
       <c r="M8" t="n">
-        <v>1585.447060299768</v>
+        <v>101962.5448758404</v>
       </c>
       <c r="N8" t="n">
-        <v>565.933839029976</v>
+        <v>13043.20566027224</v>
       </c>
       <c r="O8" t="n">
-        <v>642.9833270999831</v>
+        <v>15630.86327292188</v>
       </c>
       <c r="P8" t="n">
-        <v>1275.550950126039</v>
+        <v>84077.1471001686</v>
       </c>
       <c r="Q8" t="n">
-        <v>1449.211793384463</v>
+        <v>100757.3157190136</v>
       </c>
       <c r="R8" t="n">
-        <v>0.7529714764837523</v>
+        <v>11.40126233474416</v>
       </c>
       <c r="S8" t="n">
-        <v>0.754681956407622</v>
+        <v>11.53451147259401</v>
       </c>
       <c r="T8" t="n">
-        <v>43.21929797879984</v>
+        <v>27.11769645340559</v>
       </c>
       <c r="U8" t="n">
-        <v>43.76906446307073</v>
+        <v>25.71998407133714</v>
       </c>
       <c r="V8" t="n">
-        <v>43.22100845872372</v>
+        <v>27.25094559125544</v>
       </c>
       <c r="W8" t="n">
-        <v>43.7705675212075</v>
+        <v>25.8313361038517</v>
       </c>
       <c r="X8" t="n">
-        <v>43.22015321876178</v>
+        <v>27.18432102233051</v>
       </c>
       <c r="Y8" t="n">
-        <v>43.76981599213912</v>
+        <v>25.77566008759442</v>
       </c>
       <c r="Z8" t="n">
         <v>0</v>
       </c>
       <c r="AA8" t="n">
-        <v>5.684341886080801e-14</v>
+        <v>0</v>
       </c>
       <c r="AB8" t="n">
-        <v>0</v>
+        <v>-4.365574568510056e-11</v>
       </c>
       <c r="AC8" t="n">
-        <v>0</v>
+        <v>-7.275957614183426e-11</v>
       </c>
     </row>
     <row r="9">
@@ -1208,88 +1208,88 @@
         <v>7</v>
       </c>
       <c r="B9" t="n">
-        <v>429.3314680520052</v>
+        <v>16322.86187202349</v>
       </c>
       <c r="C9" t="n">
-        <v>1.54996678524872</v>
+        <v>5.557499003165264</v>
       </c>
       <c r="D9" t="n">
-        <v>1.466472351195947</v>
+        <v>5.011864557945529</v>
       </c>
       <c r="E9" t="n">
-        <v>42.93927315549512</v>
+        <v>13.01839398362824</v>
       </c>
       <c r="F9" t="n">
-        <v>43.44114784283002</v>
+        <v>10.6161421138269</v>
       </c>
       <c r="G9" t="n">
-        <v>371.3138463703712</v>
+        <v>1760.829253826372</v>
       </c>
       <c r="H9" t="n">
-        <v>1047.156710227632</v>
+        <v>18668.34904390513</v>
       </c>
       <c r="I9" t="n">
-        <v>117.940321739393</v>
+        <v>207.449762184769</v>
       </c>
       <c r="J9" t="n">
-        <v>0.7369729240927206</v>
+        <v>0.264252333311767</v>
       </c>
       <c r="K9" t="n">
-        <v>-160.7781547767696</v>
+        <v>-16405.35469325044</v>
       </c>
       <c r="L9" t="n">
-        <v>1585.447060299768</v>
+        <v>101962.5448758404</v>
       </c>
       <c r="M9" t="n">
-        <v>1746.225215076537</v>
+        <v>118367.8995690908</v>
       </c>
       <c r="N9" t="n">
-        <v>642.9833270999831</v>
+        <v>15630.86327292188</v>
       </c>
       <c r="O9" t="n">
-        <v>708.1874423757195</v>
+        <v>18145.80497495804</v>
       </c>
       <c r="P9" t="n">
-        <v>1449.211793384463</v>
+        <v>100757.3157190136</v>
       </c>
       <c r="Q9" t="n">
-        <v>1596.174504316629</v>
+        <v>116968.7539910089</v>
       </c>
       <c r="R9" t="n">
-        <v>0.8297913075756146</v>
+        <v>12.70159008770889</v>
       </c>
       <c r="S9" t="n">
-        <v>0.8312943657123817</v>
+        <v>12.81294212022346</v>
       </c>
       <c r="T9" t="n">
-        <v>43.76906446307073</v>
+        <v>25.71998407133714</v>
       </c>
       <c r="U9" t="n">
-        <v>44.33645792263399</v>
+        <v>24.51669348769452</v>
       </c>
       <c r="V9" t="n">
-        <v>43.7705675212075</v>
+        <v>25.8313361038517</v>
       </c>
       <c r="W9" t="n">
-        <v>44.33782054374529</v>
+        <v>24.61272232683453</v>
       </c>
       <c r="X9" t="n">
-        <v>43.76981599213912</v>
+        <v>25.77566008759442</v>
       </c>
       <c r="Y9" t="n">
-        <v>44.33713923318964</v>
+        <v>24.56470790726452</v>
       </c>
       <c r="Z9" t="n">
-        <v>2.273736754432321e-13</v>
+        <v>0</v>
       </c>
       <c r="AA9" t="n">
-        <v>5.684341886080801e-14</v>
+        <v>0</v>
       </c>
       <c r="AB9" t="n">
-        <v>0</v>
+        <v>1.455191522836685e-11</v>
       </c>
       <c r="AC9" t="n">
-        <v>0</v>
+        <v>-4.365574568510056e-11</v>
       </c>
     </row>
     <row r="10">
@@ -1297,88 +1297,88 @@
         <v>8</v>
       </c>
       <c r="B10" t="n">
-        <v>460.0153099635239</v>
+        <v>16491.98301319134</v>
       </c>
       <c r="C10" t="n">
-        <v>1.559754613942271</v>
+        <v>5.44372498324562</v>
       </c>
       <c r="D10" t="n">
-        <v>1.466472351195932</v>
+        <v>5.011864557945557</v>
       </c>
       <c r="E10" t="n">
-        <v>43.44114784283002</v>
+        <v>10.6161421138269</v>
       </c>
       <c r="F10" t="n">
-        <v>43.97248479624828</v>
+        <v>8.49056033864909</v>
       </c>
       <c r="G10" t="n">
-        <v>413.2775578681618</v>
+        <v>1901.963591663528</v>
       </c>
       <c r="H10" t="n">
-        <v>1165.500215352762</v>
+        <v>20164.65828291808</v>
       </c>
       <c r="I10" t="n">
-        <v>117.940321739393</v>
+        <v>207.449762184769</v>
       </c>
       <c r="J10" t="n">
-        <v>0.7369729240927206</v>
+        <v>0.264252333311767</v>
       </c>
       <c r="K10" t="n">
-        <v>-126.2714258508775</v>
+        <v>-15716.93509707635</v>
       </c>
       <c r="L10" t="n">
-        <v>1746.225215076537</v>
+        <v>118367.8995690908</v>
       </c>
       <c r="M10" t="n">
-        <v>1872.496640927415</v>
+        <v>134084.8346661672</v>
       </c>
       <c r="N10" t="n">
-        <v>708.1874423757195</v>
+        <v>18145.80497495804</v>
       </c>
       <c r="O10" t="n">
-        <v>759.3972389966834</v>
+        <v>20555.2119181737</v>
       </c>
       <c r="P10" t="n">
-        <v>1596.174504316629</v>
+        <v>116968.7539910089</v>
       </c>
       <c r="Q10" t="n">
-        <v>1711.595601679517</v>
+        <v>132499.9100016764</v>
       </c>
       <c r="R10" t="n">
-        <v>0.8953100798039694</v>
+        <v>13.90055137386762</v>
       </c>
       <c r="S10" t="n">
-        <v>0.8966727009152645</v>
+        <v>13.99658021300763</v>
       </c>
       <c r="T10" t="n">
-        <v>44.33645792263399</v>
+        <v>24.51669348769452</v>
       </c>
       <c r="U10" t="n">
-        <v>44.92270250451947</v>
+        <v>23.4946483694854</v>
       </c>
       <c r="V10" t="n">
-        <v>44.33782054374529</v>
+        <v>24.61272232683453</v>
       </c>
       <c r="W10" t="n">
-        <v>44.92397160924826</v>
+        <v>23.57949668928982</v>
       </c>
       <c r="X10" t="n">
-        <v>44.33713923318964</v>
+        <v>24.56470790726452</v>
       </c>
       <c r="Y10" t="n">
-        <v>44.92333705688387</v>
+        <v>23.53707252938761</v>
       </c>
       <c r="Z10" t="n">
-        <v>-2.273736754432321e-13</v>
+        <v>0</v>
       </c>
       <c r="AA10" t="n">
-        <v>0</v>
+        <v>-1.818989403545856e-12</v>
       </c>
       <c r="AB10" t="n">
-        <v>-1.13686837721616e-13</v>
+        <v>4.365574568510056e-11</v>
       </c>
       <c r="AC10" t="n">
-        <v>-1.13686837721616e-13</v>
+        <v>1.455191522836685e-11</v>
       </c>
     </row>
     <row r="11">
@@ -1386,88 +1386,88 @@
         <v>9</v>
       </c>
       <c r="B11" t="n">
-        <v>486.705313453685</v>
+        <v>16556.47195191004</v>
       </c>
       <c r="C11" t="n">
-        <v>1.570241510290336</v>
+        <v>5.34725029332284</v>
       </c>
       <c r="D11" t="n">
-        <v>1.466472351195932</v>
+        <v>5.011864557945529</v>
       </c>
       <c r="E11" t="n">
-        <v>43.97248479624828</v>
+        <v>8.49056033864909</v>
       </c>
       <c r="F11" t="n">
-        <v>44.53386404841829</v>
+        <v>6.62608620842262</v>
       </c>
       <c r="G11" t="n">
-        <v>453.385097823815</v>
+        <v>2026.343965920798</v>
       </c>
       <c r="H11" t="n">
-        <v>1278.609058467092</v>
+        <v>21483.34164520337</v>
       </c>
       <c r="I11" t="n">
-        <v>117.940321739393</v>
+        <v>207.449762184769</v>
       </c>
       <c r="J11" t="n">
-        <v>0.7369729240927206</v>
+        <v>0.264252333311767</v>
       </c>
       <c r="K11" t="n">
-        <v>-86.90491054891044</v>
+        <v>-14864.34897146451</v>
       </c>
       <c r="L11" t="n">
-        <v>1872.496640927415</v>
+        <v>134084.8346661672</v>
       </c>
       <c r="M11" t="n">
-        <v>1959.401551476325</v>
+        <v>148949.1836376316</v>
       </c>
       <c r="N11" t="n">
-        <v>759.3972389966834</v>
+        <v>20555.2119181737</v>
       </c>
       <c r="O11" t="n">
-        <v>794.6418144387039</v>
+        <v>22833.91736532472</v>
       </c>
       <c r="P11" t="n">
-        <v>1711.595601679517</v>
+        <v>132499.9100016764</v>
       </c>
       <c r="Q11" t="n">
-        <v>1791.032893799942</v>
+        <v>147188.5577212795</v>
       </c>
       <c r="R11" t="n">
-        <v>0.9502177082711901</v>
+        <v>15.00408803083631</v>
       </c>
       <c r="S11" t="n">
-        <v>0.9514868129999819</v>
+        <v>15.08893635064073</v>
       </c>
       <c r="T11" t="n">
-        <v>44.92270250451947</v>
+        <v>23.4946483694854</v>
       </c>
       <c r="U11" t="n">
-        <v>45.5292202290136</v>
+        <v>22.64297404664207</v>
       </c>
       <c r="V11" t="n">
-        <v>44.92397160924826</v>
+        <v>23.57949668928982</v>
       </c>
       <c r="W11" t="n">
-        <v>45.53043188316178</v>
+        <v>22.71940752805055</v>
       </c>
       <c r="X11" t="n">
-        <v>44.92333705688387</v>
+        <v>23.53707252938761</v>
       </c>
       <c r="Y11" t="n">
-        <v>45.52982605608769</v>
+        <v>22.68119078734631</v>
       </c>
       <c r="Z11" t="n">
-        <v>-2.273736754432321e-13</v>
+        <v>0</v>
       </c>
       <c r="AA11" t="n">
-        <v>0</v>
+        <v>-3.637978807091713e-12</v>
       </c>
       <c r="AB11" t="n">
-        <v>0</v>
+        <v>-7.275957614183426e-11</v>
       </c>
       <c r="AC11" t="n">
-        <v>0</v>
+        <v>-2.91038304567337e-11</v>
       </c>
     </row>
     <row r="12">
@@ -1475,88 +1475,88 @@
         <v>10</v>
       </c>
       <c r="B12" t="n">
-        <v>540.2860030636629</v>
+        <v>16536.19859489115</v>
       </c>
       <c r="C12" t="n">
-        <v>1.58146512122851</v>
+        <v>5.265840358557896</v>
       </c>
       <c r="D12" t="n">
-        <v>1.466472351195961</v>
+        <v>5.011864557945543</v>
       </c>
       <c r="E12" t="n">
-        <v>44.53386404841829</v>
+        <v>6.62608620842262</v>
       </c>
       <c r="F12" t="n">
-        <v>45.1259150954214</v>
+        <v>5.010018042625987</v>
       </c>
       <c r="G12" t="n">
-        <v>472.6698778669694</v>
+        <v>2134.847619650428</v>
       </c>
       <c r="H12" t="n">
-        <v>1386.376900679841</v>
+        <v>22633.69968018159</v>
       </c>
       <c r="I12" t="n">
-        <v>117.940321739393</v>
+        <v>207.449762184769</v>
       </c>
       <c r="J12" t="n">
-        <v>0.7369729240927206</v>
+        <v>0.264252333311767</v>
       </c>
       <c r="K12" t="n">
-        <v>-65.74120941342738</v>
+        <v>-13885.51036865197</v>
       </c>
       <c r="L12" t="n">
-        <v>1959.401551476325</v>
+        <v>148949.1836376316</v>
       </c>
       <c r="M12" t="n">
-        <v>2025.142760889753</v>
+        <v>162834.6940062836</v>
       </c>
       <c r="N12" t="n">
-        <v>794.6418144387039</v>
+        <v>22833.91736532472</v>
       </c>
       <c r="O12" t="n">
-        <v>821.3033805134678</v>
+        <v>24962.56680528751</v>
       </c>
       <c r="P12" t="n">
-        <v>1791.032893799942</v>
+        <v>147188.5577212795</v>
       </c>
       <c r="Q12" t="n">
-        <v>1851.125052269922</v>
+        <v>160909.9370163682</v>
       </c>
       <c r="R12" t="n">
-        <v>0.9953561805953081</v>
+        <v>16.01688783821945</v>
       </c>
       <c r="S12" t="n">
-        <v>0.9965678347434886</v>
+        <v>16.09332131962793</v>
       </c>
       <c r="T12" t="n">
-        <v>45.5292202290136</v>
+        <v>22.64297404664207</v>
       </c>
       <c r="U12" t="n">
-        <v>46.14659939473756</v>
+        <v>21.95259201409312</v>
       </c>
       <c r="V12" t="n">
-        <v>45.53043188316178</v>
+        <v>22.71940752805055</v>
       </c>
       <c r="W12" t="n">
-        <v>46.14777079247633</v>
+        <v>22.02254435686007</v>
       </c>
       <c r="X12" t="n">
-        <v>45.52982605608769</v>
+        <v>22.68119078734631</v>
       </c>
       <c r="Y12" t="n">
-        <v>46.14718509360694</v>
+        <v>21.98756818547659</v>
       </c>
       <c r="Z12" t="n">
-        <v>2.273736754432321e-13</v>
+        <v>2.91038304567337e-11</v>
       </c>
       <c r="AA12" t="n">
         <v>0</v>
       </c>
       <c r="AB12" t="n">
-        <v>-1.13686837721616e-13</v>
+        <v>-1.746229827404022e-10</v>
       </c>
       <c r="AC12" t="n">
-        <v>1.13686837721616e-13</v>
+        <v>1.01863406598568e-10</v>
       </c>
     </row>
     <row r="13">
@@ -1564,88 +1564,88 @@
         <v>11</v>
       </c>
       <c r="B13" t="n">
-        <v>610.8518413804023</v>
+        <v>16445.53165799947</v>
       </c>
       <c r="C13" t="n">
-        <v>1.593467177870363</v>
+        <v>5.197763482858588</v>
       </c>
       <c r="D13" t="n">
-        <v>1.466472351195932</v>
+        <v>5.011864557945543</v>
       </c>
       <c r="E13" t="n">
-        <v>45.1259150954214</v>
+        <v>5.010018042625987</v>
       </c>
       <c r="F13" t="n">
-        <v>45.74932103578577</v>
+        <v>3.632006118520721</v>
       </c>
       <c r="G13" t="n">
-        <v>476.9875717833157</v>
+        <v>2228.190365385293</v>
       </c>
       <c r="H13" t="n">
-        <v>1488.68834572054</v>
+        <v>23623.32144748713</v>
       </c>
       <c r="I13" t="n">
-        <v>117.940321739393</v>
+        <v>207.449762184769</v>
       </c>
       <c r="J13" t="n">
-        <v>0.7369729240927206</v>
+        <v>0.264252333311767</v>
       </c>
       <c r="K13" t="n">
-        <v>-55.73722179615582</v>
+        <v>-12810.0489584256</v>
       </c>
       <c r="L13" t="n">
-        <v>2025.142760889753</v>
+        <v>162834.6940062836</v>
       </c>
       <c r="M13" t="n">
-        <v>2080.879982685909</v>
+        <v>175644.7429647092</v>
       </c>
       <c r="N13" t="n">
-        <v>821.3033805134678</v>
+        <v>24962.56680528751</v>
       </c>
       <c r="O13" t="n">
-        <v>843.9077961456276</v>
+        <v>26926.34795681141</v>
       </c>
       <c r="P13" t="n">
-        <v>1851.125052269922</v>
+        <v>160909.9370163682</v>
       </c>
       <c r="Q13" t="n">
-        <v>1902.072851903296</v>
+        <v>173568.5671913192</v>
       </c>
       <c r="R13" t="n">
-        <v>1.020684299316151</v>
+        <v>16.94257397146713</v>
       </c>
       <c r="S13" t="n">
-        <v>1.021855697054927</v>
+        <v>17.01252631423408</v>
       </c>
       <c r="T13" t="n">
-        <v>46.14659939473756</v>
+        <v>21.95259201409312</v>
       </c>
       <c r="U13" t="n">
-        <v>46.76953706034222</v>
+        <v>21.41583731712688</v>
       </c>
       <c r="V13" t="n">
-        <v>46.14777079247633</v>
+        <v>22.02254435686007</v>
       </c>
       <c r="W13" t="n">
-        <v>46.77067625510067</v>
+        <v>21.48071327889615</v>
       </c>
       <c r="X13" t="n">
-        <v>46.14718509360694</v>
+        <v>21.98756818547659</v>
       </c>
       <c r="Y13" t="n">
-        <v>46.77010665772145</v>
+        <v>21.44827529801152</v>
       </c>
       <c r="Z13" t="n">
-        <v>0</v>
+        <v>2.91038304567337e-11</v>
       </c>
       <c r="AA13" t="n">
-        <v>-1.13686837721616e-13</v>
+        <v>0</v>
       </c>
       <c r="AB13" t="n">
-        <v>0</v>
+        <v>-6.257323548197746e-10</v>
       </c>
       <c r="AC13" t="n">
-        <v>2.273736754432321e-13</v>
+        <v>-3.92901711165905e-10</v>
       </c>
     </row>
     <row r="14">
@@ -1653,88 +1653,88 @@
         <v>12</v>
       </c>
       <c r="B14" t="n">
-        <v>677.3605753742339</v>
+        <v>16840.92743363901</v>
       </c>
       <c r="C14" t="n">
-        <v>1.606293993211679</v>
+        <v>5.061498343382219</v>
       </c>
       <c r="D14" t="n">
-        <v>1.466472351195961</v>
+        <v>4.933333333333337</v>
       </c>
       <c r="E14" t="n">
-        <v>45.74932103578577</v>
+        <v>3.632006118520721</v>
       </c>
       <c r="F14" t="n">
-        <v>46.40482325739281</v>
+        <v>2.499933806165217</v>
       </c>
       <c r="G14" t="n">
-        <v>479.3260634619982</v>
+        <v>2431.192195545536</v>
       </c>
       <c r="H14" t="n">
-        <v>1585.418165070991</v>
+        <v>25253.27239966754</v>
       </c>
       <c r="I14" t="n">
-        <v>117.940321739393</v>
+        <v>51.86244054619225</v>
       </c>
       <c r="J14" t="n">
-        <v>0.7369729240927206</v>
+        <v>0.3240724961253518</v>
       </c>
       <c r="K14" t="n">
-        <v>-41.69332443881564</v>
+        <v>-12237.44910775663</v>
       </c>
       <c r="L14" t="n">
-        <v>2080.879982685909</v>
+        <v>175644.7429647092</v>
       </c>
       <c r="M14" t="n">
-        <v>2122.573307124724</v>
+        <v>187882.1920724658</v>
       </c>
       <c r="N14" t="n">
-        <v>843.9077961456276</v>
+        <v>26926.34795681141</v>
       </c>
       <c r="O14" t="n">
-        <v>860.8166625069299</v>
+        <v>28802.34952234321</v>
       </c>
       <c r="P14" t="n">
-        <v>1902.072851903296</v>
+        <v>173568.5671913192</v>
       </c>
       <c r="Q14" t="n">
-        <v>1940.183526800704</v>
+        <v>185661.3658248471</v>
       </c>
       <c r="R14" t="n">
-        <v>1.020216024556457</v>
+        <v>17.78383119860616</v>
       </c>
       <c r="S14" t="n">
-        <v>1.021355219314905</v>
+        <v>17.84870716037543</v>
       </c>
       <c r="T14" t="n">
-        <v>46.76953706034222</v>
+        <v>21.41583731712688</v>
       </c>
       <c r="U14" t="n">
-        <v>47.40018666585145</v>
+        <v>20.96103761991525</v>
       </c>
       <c r="V14" t="n">
-        <v>46.77067625510067</v>
+        <v>21.48071327889615</v>
       </c>
       <c r="W14" t="n">
-        <v>47.40130282544054</v>
+        <v>21.02170523782245</v>
       </c>
       <c r="X14" t="n">
-        <v>46.77010665772145</v>
+        <v>21.44827529801152</v>
       </c>
       <c r="Y14" t="n">
-        <v>47.40074474564599</v>
+        <v>20.99137142886885</v>
       </c>
       <c r="Z14" t="n">
-        <v>2.273736754432321e-13</v>
+        <v>2.91038304567337e-11</v>
       </c>
       <c r="AA14" t="n">
-        <v>0</v>
+        <v>1.818989403545856e-12</v>
       </c>
       <c r="AB14" t="n">
-        <v>0</v>
+        <v>-2.91038304567337e-10</v>
       </c>
       <c r="AC14" t="n">
-        <v>0</v>
+        <v>4.365574568510056e-10</v>
       </c>
     </row>
     <row r="15">
@@ -1742,88 +1742,88 @@
         <v>13</v>
       </c>
       <c r="B15" t="n">
-        <v>740.0337169345274</v>
+        <v>17989.01218949444</v>
       </c>
       <c r="C15" t="n">
-        <v>1.619997041377506</v>
+        <v>5.017599638257071</v>
       </c>
       <c r="D15" t="n">
-        <v>1.466472351195932</v>
+        <v>4.933333333333337</v>
       </c>
       <c r="E15" t="n">
-        <v>46.40482325739281</v>
+        <v>2.499933806165217</v>
       </c>
       <c r="F15" t="n">
-        <v>47.09322675736657</v>
+        <v>1.58401478028587</v>
       </c>
       <c r="G15" t="n">
-        <v>479.6371498889574</v>
+        <v>2744.645429649843</v>
       </c>
       <c r="H15" t="n">
-        <v>1676.43041952461</v>
+        <v>28287.63820173043</v>
       </c>
       <c r="I15" t="n">
-        <v>117.940321739393</v>
+        <v>51.86244054619225</v>
       </c>
       <c r="J15" t="n">
-        <v>0.7369729240927206</v>
+        <v>0.3240724961253518</v>
       </c>
       <c r="K15" t="n">
-        <v>-24.10655213569898</v>
+        <v>-11924.9491588322</v>
       </c>
       <c r="L15" t="n">
-        <v>2122.573307124724</v>
+        <v>187882.1920724658</v>
       </c>
       <c r="M15" t="n">
-        <v>2146.679859260423</v>
+        <v>199807.141231298</v>
       </c>
       <c r="N15" t="n">
-        <v>860.8166625069299</v>
+        <v>28802.34952234321</v>
       </c>
       <c r="O15" t="n">
-        <v>870.5931548826452</v>
+        <v>30630.44482994099</v>
       </c>
       <c r="P15" t="n">
-        <v>1940.183526800704</v>
+        <v>185661.3658248471</v>
       </c>
       <c r="Q15" t="n">
-        <v>1962.21863634658</v>
+        <v>197445.3583565433</v>
       </c>
       <c r="R15" t="n">
-        <v>0.9953634084586437</v>
+        <v>18.46110381375004</v>
       </c>
       <c r="S15" t="n">
-        <v>0.9964795680477334</v>
+        <v>18.52177143165724</v>
       </c>
       <c r="T15" t="n">
-        <v>47.40018666585145</v>
+        <v>20.96103761991525</v>
       </c>
       <c r="U15" t="n">
-        <v>48.03986273062048</v>
+        <v>20.5743867053862</v>
       </c>
       <c r="V15" t="n">
-        <v>47.40130282544054</v>
+        <v>21.02170523782245</v>
       </c>
       <c r="W15" t="n">
-        <v>48.04096594726346</v>
+        <v>20.63144590002306</v>
       </c>
       <c r="X15" t="n">
-        <v>47.40074474564599</v>
+        <v>20.99137142886885</v>
       </c>
       <c r="Y15" t="n">
-        <v>48.04041433894197</v>
+        <v>20.60291630270463</v>
       </c>
       <c r="Z15" t="n">
-        <v>0</v>
+        <v>-2.91038304567337e-11</v>
       </c>
       <c r="AA15" t="n">
         <v>0</v>
       </c>
       <c r="AB15" t="n">
-        <v>0</v>
+        <v>-7.275957614183426e-11</v>
       </c>
       <c r="AC15" t="n">
-        <v>0</v>
+        <v>-7.275957614183426e-11</v>
       </c>
     </row>
     <row r="16">
@@ -1831,88 +1831,88 @@
         <v>14</v>
       </c>
       <c r="B16" t="n">
-        <v>799.0783153918494</v>
+        <v>18994.21585238587</v>
       </c>
       <c r="C16" t="n">
-        <v>1.63463363420544</v>
+        <v>4.983395874270569</v>
       </c>
       <c r="D16" t="n">
-        <v>1.466472351195932</v>
+        <v>4.933333333333337</v>
       </c>
       <c r="E16" t="n">
-        <v>47.09322675736657</v>
+        <v>1.58401478028587</v>
       </c>
       <c r="F16" t="n">
-        <v>47.81540619668814</v>
+        <v>0.8792629304200403</v>
       </c>
       <c r="G16" t="n">
-        <v>477.8684761037409</v>
+        <v>3044.776535253171</v>
       </c>
       <c r="H16" t="n">
-        <v>1761.577460808501</v>
+        <v>31182.97563712927</v>
       </c>
       <c r="I16" t="n">
-        <v>117.940321739393</v>
+        <v>51.86244054619225</v>
       </c>
       <c r="J16" t="n">
-        <v>0.7369729240927206</v>
+        <v>0.3240724961253518</v>
       </c>
       <c r="K16" t="n">
-        <v>-3.470649621458456</v>
+        <v>-11314.16819253878</v>
       </c>
       <c r="L16" t="n">
-        <v>2146.679859260423</v>
+        <v>199807.141231298</v>
       </c>
       <c r="M16" t="n">
-        <v>2150.150508881881</v>
+        <v>211121.3094238368</v>
       </c>
       <c r="N16" t="n">
-        <v>870.5931548826452</v>
+        <v>30630.44482994099</v>
       </c>
       <c r="O16" t="n">
-        <v>872.0006883769404</v>
+        <v>32364.9073845954</v>
       </c>
       <c r="P16" t="n">
-        <v>1962.21863634658</v>
+        <v>197445.3583565433</v>
       </c>
       <c r="Q16" t="n">
-        <v>1965.391057859772</v>
+        <v>208625.7895439152</v>
       </c>
       <c r="R16" t="n">
-        <v>0.9466359732539136</v>
+        <v>18.99037192510033</v>
       </c>
       <c r="S16" t="n">
-        <v>0.9477391898968907</v>
+        <v>19.04743111973719</v>
       </c>
       <c r="T16" t="n">
-        <v>48.03986273062048</v>
+        <v>20.5743867053862</v>
       </c>
       <c r="U16" t="n">
-        <v>48.68903394945598</v>
+        <v>20.28260785724047</v>
       </c>
       <c r="V16" t="n">
-        <v>48.04096594726346</v>
+        <v>20.63144590002306</v>
       </c>
       <c r="W16" t="n">
-        <v>48.69013532144522</v>
+        <v>20.3366175105607</v>
       </c>
       <c r="X16" t="n">
-        <v>48.04041433894197</v>
+        <v>20.60291630270463</v>
       </c>
       <c r="Y16" t="n">
-        <v>48.6895846354506</v>
+        <v>20.30961268390058</v>
       </c>
       <c r="Z16" t="n">
-        <v>-2.273736754432321e-13</v>
+        <v>0</v>
       </c>
       <c r="AA16" t="n">
         <v>0</v>
       </c>
       <c r="AB16" t="n">
-        <v>0</v>
+        <v>-2.037268131971359e-10</v>
       </c>
       <c r="AC16" t="n">
-        <v>0</v>
+        <v>6.111804395914078e-10</v>
       </c>
     </row>
     <row r="17">
@@ -1920,88 +1920,88 @@
         <v>15</v>
       </c>
       <c r="B17" t="n">
-        <v>854.6887040459757</v>
+        <v>20168.14916496954</v>
       </c>
       <c r="C17" t="n">
-        <v>1.650267714633164</v>
+        <v>4.958325873137537</v>
       </c>
       <c r="D17" t="n">
-        <v>1.466472351195961</v>
+        <v>4.933333333333337</v>
       </c>
       <c r="E17" t="n">
-        <v>47.81540619668814</v>
+        <v>0.8792629304200403</v>
       </c>
       <c r="F17" t="n">
-        <v>48.57231281173381</v>
+        <v>0.3819458071278916</v>
       </c>
       <c r="G17" t="n">
-        <v>473.96313169945</v>
+        <v>3278.096587903534</v>
       </c>
       <c r="H17" t="n">
-        <v>1840.698793656881</v>
+        <v>33942.11362248049</v>
       </c>
       <c r="I17" t="n">
-        <v>117.940321739393</v>
+        <v>51.86244054619225</v>
       </c>
       <c r="J17" t="n">
-        <v>0.7369729240927206</v>
+        <v>0.3240724961253518</v>
       </c>
       <c r="K17" t="n">
-        <v>19.7196798423448</v>
+        <v>-10535.70722439512</v>
       </c>
       <c r="L17" t="n">
-        <v>2150.150508881881</v>
+        <v>211121.3094238368</v>
       </c>
       <c r="M17" t="n">
-        <v>2130.430829039537</v>
+        <v>221657.0166482319</v>
       </c>
       <c r="N17" t="n">
-        <v>872.0006883769404</v>
+        <v>32364.9073845954</v>
       </c>
       <c r="O17" t="n">
-        <v>864.0033066466542</v>
+        <v>33980.03183356427</v>
       </c>
       <c r="P17" t="n">
-        <v>1965.391057859772</v>
+        <v>208625.7895439152</v>
       </c>
       <c r="Q17" t="n">
-        <v>1947.365862755567</v>
+        <v>219036.9614151559</v>
       </c>
       <c r="R17" t="n">
-        <v>0.8736277527678384</v>
+        <v>19.40334492682043</v>
       </c>
       <c r="S17" t="n">
-        <v>0.8747291247570748</v>
+        <v>19.45735458014066</v>
       </c>
       <c r="T17" t="n">
-        <v>48.68903394945598</v>
+        <v>20.28260785724047</v>
       </c>
       <c r="U17" t="n">
-        <v>49.34726986811383</v>
+        <v>20.09565267968819</v>
       </c>
       <c r="V17" t="n">
-        <v>48.69013532144522</v>
+        <v>20.3366175105607</v>
       </c>
       <c r="W17" t="n">
-        <v>49.34838183360162</v>
+        <v>20.14710026549978</v>
       </c>
       <c r="X17" t="n">
-        <v>48.6895846354506</v>
+        <v>20.30961268390058</v>
       </c>
       <c r="Y17" t="n">
-        <v>49.34782585085772</v>
+        <v>20.12137647259399</v>
       </c>
       <c r="Z17" t="n">
-        <v>0</v>
+        <v>2.91038304567337e-11</v>
       </c>
       <c r="AA17" t="n">
-        <v>0</v>
+        <v>-3.637978807091713e-12</v>
       </c>
       <c r="AB17" t="n">
-        <v>0</v>
+        <v>3.346940502524376e-10</v>
       </c>
       <c r="AC17" t="n">
-        <v>0</v>
+        <v>2.764863893389702e-10</v>
       </c>
     </row>
     <row r="18">
@@ -2009,88 +2009,88 @@
         <v>16</v>
       </c>
       <c r="B18" t="n">
-        <v>907.0481677354268</v>
+        <v>21511.01192419735</v>
       </c>
       <c r="C18" t="n">
-        <v>1.666970791043669</v>
+        <v>4.941991117525683</v>
       </c>
       <c r="D18" t="n">
-        <v>1.466472351195932</v>
+        <v>4.933333333333337</v>
       </c>
       <c r="E18" t="n">
-        <v>48.57231281173381</v>
+        <v>0.3819458071278916</v>
       </c>
       <c r="F18" t="n">
-        <v>49.36498233025576</v>
+        <v>0.08948243701796343</v>
       </c>
       <c r="G18" t="n">
-        <v>467.8591894675404</v>
+        <v>3444.801909328067</v>
       </c>
       <c r="H18" t="n">
-        <v>1913.619774725184</v>
+        <v>36567.10095119293</v>
       </c>
       <c r="I18" t="n">
-        <v>117.940321739393</v>
+        <v>51.86244054619225</v>
       </c>
       <c r="J18" t="n">
-        <v>0.7369729240927206</v>
+        <v>0.3240724961253518</v>
       </c>
       <c r="K18" t="n">
-        <v>44.96431075206866</v>
+        <v>-9608.341939120943</v>
       </c>
       <c r="L18" t="n">
-        <v>2130.430829039537</v>
+        <v>221657.0166482319</v>
       </c>
       <c r="M18" t="n">
-        <v>2085.466518287468</v>
+        <v>231265.3585873529</v>
       </c>
       <c r="N18" t="n">
-        <v>864.0033066466542</v>
+        <v>33980.03183356427</v>
       </c>
       <c r="O18" t="n">
-        <v>845.7678809096029</v>
+        <v>35452.99113752008</v>
       </c>
       <c r="P18" t="n">
-        <v>1947.365862755567</v>
+        <v>219036.9614151559</v>
       </c>
       <c r="Q18" t="n">
-        <v>1906.265272862026</v>
+        <v>228531.7297487153</v>
       </c>
       <c r="R18" t="n">
-        <v>0.7749570563800198</v>
+        <v>19.7137068725603</v>
       </c>
       <c r="S18" t="n">
-        <v>0.7760690218678155</v>
+        <v>19.76515445837189</v>
       </c>
       <c r="T18" t="n">
-        <v>49.34726986811383</v>
+        <v>20.09565267968819</v>
       </c>
       <c r="U18" t="n">
-        <v>50.01308838704362</v>
+        <v>20.01996214938983</v>
       </c>
       <c r="V18" t="n">
-        <v>49.34838183360162</v>
+        <v>20.14710026549978</v>
       </c>
       <c r="W18" t="n">
-        <v>50.01422534068451</v>
+        <v>20.06927483660776</v>
       </c>
       <c r="X18" t="n">
-        <v>49.34782585085772</v>
+        <v>20.12137647259399</v>
       </c>
       <c r="Y18" t="n">
-        <v>50.01365686386406</v>
+        <v>20.0446184929988</v>
       </c>
       <c r="Z18" t="n">
-        <v>-2.273736754432321e-13</v>
+        <v>-2.91038304567337e-11</v>
       </c>
       <c r="AA18" t="n">
-        <v>-1.13686837721616e-13</v>
+        <v>-3.637978807091713e-12</v>
       </c>
       <c r="AB18" t="n">
-        <v>0</v>
+        <v>1.455191522836685e-11</v>
       </c>
       <c r="AC18" t="n">
-        <v>0</v>
+        <v>-2.764863893389702e-10</v>
       </c>
     </row>
     <row r="19">
@@ -2098,88 +2098,88 @@
         <v>17</v>
       </c>
       <c r="B19" t="n">
-        <v>956.3305665821792</v>
+        <v>22743.03077422489</v>
       </c>
       <c r="C19" t="n">
-        <v>1.684823042688945</v>
+        <v>4.934137670953151</v>
       </c>
       <c r="D19" t="n">
-        <v>1.466472351195932</v>
+        <v>4.933333333333337</v>
       </c>
       <c r="E19" t="n">
-        <v>49.36498233025576</v>
+        <v>0.08948243701796343</v>
       </c>
       <c r="F19" t="n">
-        <v>50.19454407086326</v>
+        <v>0.000375000585933094</v>
       </c>
       <c r="G19" t="n">
-        <v>459.4891760530703</v>
+        <v>3598.779344952007</v>
       </c>
       <c r="H19" t="n">
-        <v>1980.150119764548</v>
+        <v>39059.26136911457</v>
       </c>
       <c r="I19" t="n">
-        <v>117.940321739393</v>
+        <v>51.86244054619225</v>
       </c>
       <c r="J19" t="n">
-        <v>0.7369729240927206</v>
+        <v>0.3240724961253518</v>
       </c>
       <c r="K19" t="n">
-        <v>71.75290996477646</v>
+        <v>-8456.247728299566</v>
       </c>
       <c r="L19" t="n">
-        <v>2085.466518287468</v>
+        <v>231265.3585873529</v>
       </c>
       <c r="M19" t="n">
-        <v>2013.713608322691</v>
+        <v>239721.6063156525</v>
       </c>
       <c r="N19" t="n">
-        <v>845.7678809096029</v>
+        <v>35452.99113752008</v>
       </c>
       <c r="O19" t="n">
-        <v>816.6682496866376</v>
+        <v>36749.33434084009</v>
       </c>
       <c r="P19" t="n">
-        <v>1906.265272862026</v>
+        <v>228531.7297487153</v>
       </c>
       <c r="Q19" t="n">
-        <v>1840.677990930993</v>
+        <v>236888.0219852026</v>
       </c>
       <c r="R19" t="n">
-        <v>0.6481060567878625</v>
+        <v>19.93047971237187</v>
       </c>
       <c r="S19" t="n">
-        <v>0.6492430104287549</v>
+        <v>19.9797923995898</v>
       </c>
       <c r="T19" t="n">
-        <v>50.01308838704362</v>
+        <v>20.01996214938983</v>
       </c>
       <c r="U19" t="n">
-        <v>50.68363467394698</v>
+        <v>20.06716493291046</v>
       </c>
       <c r="V19" t="n">
-        <v>50.01422534068451</v>
+        <v>20.06927483660776</v>
       </c>
       <c r="W19" t="n">
-        <v>50.68481396851657</v>
+        <v>20.11473876564636</v>
       </c>
       <c r="X19" t="n">
-        <v>50.01365686386406</v>
+        <v>20.0446184929988</v>
       </c>
       <c r="Y19" t="n">
-        <v>50.68422432123178</v>
+        <v>20.09095184927841</v>
       </c>
       <c r="Z19" t="n">
-        <v>0</v>
+        <v>-2.91038304567337e-11</v>
       </c>
       <c r="AA19" t="n">
-        <v>1.13686837721616e-13</v>
+        <v>-3.637978807091713e-12</v>
       </c>
       <c r="AB19" t="n">
-        <v>0</v>
+        <v>1.746229827404022e-10</v>
       </c>
       <c r="AC19" t="n">
-        <v>0</v>
+        <v>-3.783497959375381e-10</v>
       </c>
     </row>
     <row r="20">
@@ -2187,88 +2187,88 @@
         <v>18</v>
       </c>
       <c r="B20" t="n">
-        <v>1002.701953472272</v>
+        <v>23889.38529501095</v>
       </c>
       <c r="C20" t="n">
-        <v>1.703914634042265</v>
+        <v>4.941316641688443</v>
       </c>
       <c r="D20" t="n">
-        <v>1.466472351195961</v>
+        <v>4.939999999999998</v>
       </c>
       <c r="E20" t="n">
-        <v>50.19454407086326</v>
+        <v>0.000375000585933094</v>
       </c>
       <c r="F20" t="n">
-        <v>51.06223144461947</v>
+        <v>0.1144612557461073</v>
       </c>
       <c r="G20" t="n">
-        <v>448.7794622838701</v>
+        <v>3740.180780181216</v>
       </c>
       <c r="H20" t="n">
-        <v>2040.082184264922</v>
+        <v>41573.94995289368</v>
       </c>
       <c r="I20" t="n">
-        <v>117.940321739393</v>
+        <v>103.7248810923845</v>
       </c>
       <c r="J20" t="n">
-        <v>0.7369729240927206</v>
+        <v>0.2757574878739312</v>
       </c>
       <c r="K20" t="n">
-        <v>99.55970521061151</v>
+        <v>-6193.471869835437</v>
       </c>
       <c r="L20" t="n">
-        <v>2013.713608322691</v>
+        <v>239721.6063156525</v>
       </c>
       <c r="M20" t="n">
-        <v>1914.15390311208</v>
+        <v>245915.0781854879</v>
       </c>
       <c r="N20" t="n">
-        <v>816.6682496866376</v>
+        <v>36749.33434084009</v>
       </c>
       <c r="O20" t="n">
-        <v>776.2914801909038</v>
+        <v>37698.79389091281</v>
       </c>
       <c r="P20" t="n">
-        <v>1840.677990930993</v>
+        <v>236888.0219852026</v>
       </c>
       <c r="Q20" t="n">
-        <v>1749.673313102256</v>
+        <v>243008.2850812809</v>
       </c>
       <c r="R20" t="n">
-        <v>0.4890906030837232</v>
+        <v>20.06678993232453</v>
       </c>
       <c r="S20" t="n">
-        <v>0.4902698976533119</v>
+        <v>20.11436376506043</v>
       </c>
       <c r="T20" t="n">
-        <v>50.68363467394698</v>
+        <v>20.06716493291046</v>
       </c>
       <c r="U20" t="n">
-        <v>51.35406889948894</v>
+        <v>20.31992189476758</v>
       </c>
       <c r="V20" t="n">
-        <v>50.68481396851657</v>
+        <v>20.11473876564636</v>
       </c>
       <c r="W20" t="n">
-        <v>51.35531245298841</v>
+        <v>20.36629695168282</v>
       </c>
       <c r="X20" t="n">
-        <v>50.68422432123178</v>
+        <v>20.09095184927841</v>
       </c>
       <c r="Y20" t="n">
-        <v>51.35469067623868</v>
+        <v>20.3431094232252</v>
       </c>
       <c r="Z20" t="n">
-        <v>0</v>
+        <v>5.820766091346741e-11</v>
       </c>
       <c r="AA20" t="n">
-        <v>-1.13686837721616e-13</v>
+        <v>0</v>
       </c>
       <c r="AB20" t="n">
-        <v>0</v>
+        <v>8.731149137020111e-11</v>
       </c>
       <c r="AC20" t="n">
-        <v>0</v>
+        <v>-1.455191522836685e-10</v>
       </c>
     </row>
     <row r="21">
@@ -2276,88 +2276,88 @@
         <v>19</v>
       </c>
       <c r="B21" t="n">
-        <v>1046.322227192165</v>
+        <v>25313.23045581872</v>
       </c>
       <c r="C21" t="n">
-        <v>1.724347285969732</v>
+        <v>4.950227991703982</v>
       </c>
       <c r="D21" t="n">
-        <v>1.466472351195932</v>
+        <v>4.939999999999998</v>
       </c>
       <c r="E21" t="n">
-        <v>51.06223144461947</v>
+        <v>0.1144612557461073</v>
       </c>
       <c r="F21" t="n">
-        <v>51.96939412734315</v>
+        <v>0.4325813609744245</v>
       </c>
       <c r="G21" t="n">
-        <v>435.6495580652557</v>
+        <v>3841.659750710529</v>
       </c>
       <c r="H21" t="n">
-        <v>2093.188974960039</v>
+        <v>44001.92335492501</v>
       </c>
       <c r="I21" t="n">
-        <v>117.940321739393</v>
+        <v>103.7248810923845</v>
       </c>
       <c r="J21" t="n">
-        <v>0.7369729240927206</v>
+        <v>0.2757574878739312</v>
       </c>
       <c r="K21" t="n">
-        <v>127.8376586491104</v>
+        <v>-4685.45156773721</v>
       </c>
       <c r="L21" t="n">
-        <v>1914.15390311208</v>
+        <v>245915.0781854879</v>
       </c>
       <c r="M21" t="n">
-        <v>1786.316244462969</v>
+        <v>250600.5297532251</v>
       </c>
       <c r="N21" t="n">
-        <v>776.2914801909038</v>
+        <v>37698.79389091281</v>
       </c>
       <c r="O21" t="n">
-        <v>724.4464926507109</v>
+        <v>38417.07385260246</v>
       </c>
       <c r="P21" t="n">
-        <v>1749.673313102256</v>
+        <v>243008.2850812809</v>
       </c>
       <c r="Q21" t="n">
-        <v>1632.820567153161</v>
+        <v>247638.3531466819</v>
       </c>
       <c r="R21" t="n">
-        <v>0.2918374548694682</v>
+        <v>20.20546063902147</v>
       </c>
       <c r="S21" t="n">
-        <v>0.2930810083689363</v>
+        <v>20.25183569593672</v>
       </c>
       <c r="T21" t="n">
-        <v>51.35406889948894</v>
+        <v>20.31992189476758</v>
       </c>
       <c r="U21" t="n">
-        <v>52.01641452289101</v>
+        <v>20.70431369133387</v>
       </c>
       <c r="V21" t="n">
-        <v>51.35531245298841</v>
+        <v>20.36629695168282</v>
       </c>
       <c r="W21" t="n">
-        <v>52.01775147841057</v>
+        <v>20.74982040816116</v>
       </c>
       <c r="X21" t="n">
-        <v>51.35469067623868</v>
+        <v>20.3431094232252</v>
       </c>
       <c r="Y21" t="n">
-        <v>52.01708300065079</v>
+        <v>20.72706704974752</v>
       </c>
       <c r="Z21" t="n">
-        <v>0</v>
+        <v>-2.91038304567337e-11</v>
       </c>
       <c r="AA21" t="n">
         <v>0</v>
       </c>
       <c r="AB21" t="n">
-        <v>0</v>
+        <v>-3.783497959375381e-10</v>
       </c>
       <c r="AC21" t="n">
-        <v>0</v>
+        <v>2.91038304567337e-10</v>
       </c>
     </row>
     <row r="22">
@@ -2365,88 +2365,88 @@
         <v>20</v>
       </c>
       <c r="B22" t="n">
-        <v>1071.929397845538</v>
+        <v>26771.14991922581</v>
       </c>
       <c r="C22" t="n">
-        <v>1.730020045640405</v>
+        <v>4.967679211374814</v>
       </c>
       <c r="D22" t="n">
-        <v>1.452941176470574</v>
+        <v>4.939999999999998</v>
       </c>
       <c r="E22" t="n">
-        <v>51.96939412734315</v>
+        <v>0.4325813609744245</v>
       </c>
       <c r="F22" t="n">
-        <v>52.90857190738048</v>
+        <v>0.9563710230572724</v>
       </c>
       <c r="G22" t="n">
-        <v>420.0893443037693</v>
+        <v>3907.885915200318</v>
       </c>
       <c r="H22" t="n">
-        <v>2127.697389360855</v>
+        <v>46296.4042138433</v>
       </c>
       <c r="I22" t="n">
-        <v>235.880643478786</v>
+        <v>103.7248810923845</v>
       </c>
       <c r="J22" t="n">
-        <v>0.627099814420246</v>
+        <v>0.2757574878739312</v>
       </c>
       <c r="K22" t="n">
-        <v>75.62029014302229</v>
+        <v>-3020.726314514223</v>
       </c>
       <c r="L22" t="n">
-        <v>1786.316244462969</v>
+        <v>250600.5297532251</v>
       </c>
       <c r="M22" t="n">
-        <v>1710.695954319947</v>
+        <v>253621.2560677393</v>
       </c>
       <c r="N22" t="n">
-        <v>724.4464926507109</v>
+        <v>38417.07385260246</v>
       </c>
       <c r="O22" t="n">
-        <v>693.7784325369704</v>
+        <v>38880.1513489967</v>
       </c>
       <c r="P22" t="n">
-        <v>1632.820567153161</v>
+        <v>247638.3531466819</v>
       </c>
       <c r="Q22" t="n">
-        <v>1563.698223658638</v>
+        <v>250623.3735317935</v>
       </c>
       <c r="R22" t="n">
-        <v>0.04702039554785751</v>
+        <v>20.27173233035944</v>
       </c>
       <c r="S22" t="n">
-        <v>0.04835735106741525</v>
+        <v>20.31723904718674</v>
       </c>
       <c r="T22" t="n">
-        <v>52.01641452289101</v>
+        <v>20.70431369133387</v>
       </c>
       <c r="U22" t="n">
-        <v>52.65661957107645</v>
+        <v>21.22778658584512</v>
       </c>
       <c r="V22" t="n">
-        <v>52.01775147841057</v>
+        <v>20.74982040816116</v>
       </c>
       <c r="W22" t="n">
-        <v>52.65801853491705</v>
+        <v>21.27274994869163</v>
       </c>
       <c r="X22" t="n">
-        <v>52.01708300065079</v>
+        <v>20.72706704974752</v>
       </c>
       <c r="Y22" t="n">
-        <v>52.65731905299675</v>
+        <v>21.25026826726837</v>
       </c>
       <c r="Z22" t="n">
-        <v>-2.273736754432321e-13</v>
+        <v>-2.91038304567337e-11</v>
       </c>
       <c r="AA22" t="n">
-        <v>0</v>
+        <v>3.637978807091713e-12</v>
       </c>
       <c r="AB22" t="n">
-        <v>0</v>
+        <v>-1.164153218269348e-10</v>
       </c>
       <c r="AC22" t="n">
-        <v>0</v>
+        <v>3.783497959375381e-10</v>
       </c>
     </row>
     <row r="23">
@@ -2454,88 +2454,88 @@
         <v>21</v>
       </c>
       <c r="B23" t="n">
-        <v>1122.598021402422</v>
+        <v>28158.56862926312</v>
       </c>
       <c r="C23" t="n">
-        <v>1.753049692282183</v>
+        <v>4.993942948563728</v>
       </c>
       <c r="D23" t="n">
-        <v>1.452941176470603</v>
+        <v>4.939999999999998</v>
       </c>
       <c r="E23" t="n">
-        <v>52.90857190738048</v>
+        <v>0.9563710230572724</v>
       </c>
       <c r="F23" t="n">
-        <v>53.88953436174755</v>
+        <v>1.688561837834129</v>
       </c>
       <c r="G23" t="n">
-        <v>402.038608381131</v>
+        <v>3961.201858380001</v>
       </c>
       <c r="H23" t="n">
-        <v>2182.55701130716</v>
+        <v>48455.97326007098</v>
       </c>
       <c r="I23" t="n">
-        <v>235.880643478786</v>
+        <v>103.7248810923845</v>
       </c>
       <c r="J23" t="n">
-        <v>0.627099814420246</v>
+        <v>0.2757574878739312</v>
       </c>
       <c r="K23" t="n">
-        <v>105.3541297941052</v>
+        <v>-1180.121412696659</v>
       </c>
       <c r="L23" t="n">
-        <v>1710.695954319947</v>
+        <v>253621.2560677393</v>
       </c>
       <c r="M23" t="n">
-        <v>1605.341824525842</v>
+        <v>254801.377480436</v>
       </c>
       <c r="N23" t="n">
-        <v>693.7784325369704</v>
+        <v>38880.1513489967</v>
       </c>
       <c r="O23" t="n">
-        <v>651.0517148842666</v>
+        <v>39061.0640210938</v>
       </c>
       <c r="P23" t="n">
-        <v>1563.698223658638</v>
+        <v>250623.3735317935</v>
       </c>
       <c r="Q23" t="n">
-        <v>1467.397028114141</v>
+        <v>251789.5455404526</v>
       </c>
       <c r="R23" t="n">
-        <v>-0.2519523363040272</v>
+        <v>20.27141556278784</v>
       </c>
       <c r="S23" t="n">
-        <v>-0.2505533724634326</v>
+        <v>20.31637892563436</v>
       </c>
       <c r="T23" t="n">
-        <v>52.65661957107645</v>
+        <v>21.22778658584512</v>
       </c>
       <c r="U23" t="n">
-        <v>53.27368421116554</v>
+        <v>21.90018094152369</v>
       </c>
       <c r="V23" t="n">
-        <v>52.65801853491705</v>
+        <v>21.27274994869163</v>
       </c>
       <c r="W23" t="n">
-        <v>53.27517974113</v>
+        <v>21.94493530464943</v>
       </c>
       <c r="X23" t="n">
-        <v>52.65731905299675</v>
+        <v>21.25026826726837</v>
       </c>
       <c r="Y23" t="n">
-        <v>53.27443197614777</v>
+        <v>21.92255812308656</v>
       </c>
       <c r="Z23" t="n">
-        <v>2.273736754432321e-13</v>
+        <v>0</v>
       </c>
       <c r="AA23" t="n">
-        <v>1.13686837721616e-13</v>
+        <v>-3.637978807091713e-12</v>
       </c>
       <c r="AB23" t="n">
-        <v>0</v>
+        <v>-5.093170329928398e-10</v>
       </c>
       <c r="AC23" t="n">
-        <v>0</v>
+        <v>8.294591680169106e-10</v>
       </c>
     </row>
     <row r="24">
@@ -2543,88 +2543,88 @@
         <v>22</v>
       </c>
       <c r="B24" t="n">
-        <v>1170.791521405582</v>
+        <v>29484.86043834919</v>
       </c>
       <c r="C24" t="n">
-        <v>1.777766065969487</v>
+        <v>5.029439281290534</v>
       </c>
       <c r="D24" t="n">
-        <v>1.452941176470574</v>
+        <v>4.939999999999998</v>
       </c>
       <c r="E24" t="n">
-        <v>53.88953436174755</v>
+        <v>1.688561837834129</v>
       </c>
       <c r="F24" t="n">
-        <v>54.9140235655541</v>
+        <v>2.633054056944971</v>
       </c>
       <c r="G24" t="n">
-        <v>381.3274867664382</v>
+        <v>4001.401361654634</v>
       </c>
       <c r="H24" t="n">
-        <v>2229.983202643226</v>
+        <v>50478.4755092909</v>
       </c>
       <c r="I24" t="n">
-        <v>235.880643478786</v>
+        <v>103.7248810923845</v>
       </c>
       <c r="J24" t="n">
-        <v>0.627099814420246</v>
+        <v>0.2757574878739312</v>
       </c>
       <c r="K24" t="n">
-        <v>134.0282867299974</v>
+        <v>825.4892950511562</v>
       </c>
       <c r="L24" t="n">
-        <v>1605.341824525842</v>
+        <v>254801.377480436</v>
       </c>
       <c r="M24" t="n">
-        <v>1471.313537795844</v>
+        <v>253975.8881853848</v>
       </c>
       <c r="N24" t="n">
-        <v>651.0517148842666</v>
+        <v>39061.0640210938</v>
       </c>
       <c r="O24" t="n">
-        <v>596.6960975413135</v>
+        <v>38934.51647052101</v>
       </c>
       <c r="P24" t="n">
-        <v>1467.397028114141</v>
+        <v>251789.5455404526</v>
       </c>
       <c r="Q24" t="n">
-        <v>1344.8856061689</v>
+        <v>250973.8137869404</v>
       </c>
       <c r="R24" t="n">
-        <v>-0.6158501505820028</v>
+        <v>20.21161910368956</v>
       </c>
       <c r="S24" t="n">
-        <v>-0.6143546206175524</v>
+        <v>20.2563734668153</v>
       </c>
       <c r="T24" t="n">
-        <v>53.27368421116554</v>
+        <v>21.90018094152369</v>
       </c>
       <c r="U24" t="n">
-        <v>53.84491695264224</v>
+        <v>22.73194512569428</v>
       </c>
       <c r="V24" t="n">
-        <v>53.27517974113</v>
+        <v>21.94493530464943</v>
       </c>
       <c r="W24" t="n">
-        <v>53.84655600858774</v>
+        <v>22.77684565119949</v>
       </c>
       <c r="X24" t="n">
-        <v>53.27443197614777</v>
+        <v>21.92255812308656</v>
       </c>
       <c r="Y24" t="n">
-        <v>53.84573648061499</v>
+        <v>22.75439538844689</v>
       </c>
       <c r="Z24" t="n">
         <v>0</v>
       </c>
       <c r="AA24" t="n">
-        <v>0</v>
+        <v>3.637978807091713e-12</v>
       </c>
       <c r="AB24" t="n">
-        <v>0</v>
+        <v>7.275957614183426e-11</v>
       </c>
       <c r="AC24" t="n">
-        <v>2.273736754432321e-13</v>
+        <v>-3.92901711165905e-10</v>
       </c>
     </row>
     <row r="25">
@@ -2632,76 +2632,76 @@
         <v>23</v>
       </c>
       <c r="B25" t="n">
-        <v>1222.807269067328</v>
+        <v>29686.56913536489</v>
       </c>
       <c r="C25" t="n">
-        <v>1.804333835711337</v>
+        <v>5.105586415396622</v>
       </c>
       <c r="D25" t="n">
-        <v>1.452941176470603</v>
+        <v>4.96986335153602</v>
       </c>
       <c r="E25" t="n">
-        <v>54.9140235655541</v>
+        <v>2.633054056944971</v>
       </c>
       <c r="F25" t="n">
-        <v>55.98396391222813</v>
+        <v>3.802722533226884</v>
       </c>
       <c r="G25" t="n">
-        <v>353.9580076876129</v>
+        <v>4028.262570232269</v>
       </c>
       <c r="H25" t="n">
-        <v>2269.656855390149</v>
+        <v>51383.02642826504</v>
       </c>
       <c r="I25" t="n">
-        <v>235.880643478786</v>
+        <v>103.7248810923845</v>
       </c>
       <c r="J25" t="n">
-        <v>0.627099814420246</v>
+        <v>0.2757574878739312</v>
       </c>
       <c r="K25" t="n">
-        <v>157.0142282198798</v>
+        <v>3062.071509401099</v>
       </c>
       <c r="L25" t="n">
-        <v>1471.313537795844</v>
+        <v>253975.8881853848</v>
       </c>
       <c r="M25" t="n">
-        <v>1314.299309575965</v>
+        <v>250913.8166759837</v>
       </c>
       <c r="N25" t="n">
-        <v>596.6960975413135</v>
+        <v>38934.51647052101</v>
       </c>
       <c r="O25" t="n">
-        <v>533.0184551962163</v>
+        <v>38465.10075366498</v>
       </c>
       <c r="P25" t="n">
-        <v>1344.8856061689</v>
+        <v>250973.8137869404</v>
       </c>
       <c r="Q25" t="n">
-        <v>1201.363392805065</v>
+        <v>247947.9369200711</v>
       </c>
       <c r="R25" t="n">
-        <v>-1.069106612911859</v>
+        <v>20.09889106874931</v>
       </c>
       <c r="S25" t="n">
-        <v>-1.067467556966361</v>
+        <v>20.14379159425452</v>
       </c>
       <c r="T25" t="n">
-        <v>53.84491695264224</v>
+        <v>22.73194512569428</v>
       </c>
       <c r="U25" t="n">
-        <v>54.33642300537958</v>
+        <v>23.74578486216365</v>
       </c>
       <c r="V25" t="n">
-        <v>53.84655600858774</v>
+        <v>22.77684565119949</v>
       </c>
       <c r="W25" t="n">
-        <v>54.33826847058606</v>
+        <v>23.79123674842312</v>
       </c>
       <c r="X25" t="n">
-        <v>53.84573648061499</v>
+        <v>22.75439538844689</v>
       </c>
       <c r="Y25" t="n">
-        <v>54.33734573798282</v>
+        <v>23.76851080529338</v>
       </c>
       <c r="Z25" t="n">
         <v>0</v>
@@ -2710,10 +2710,10 @@
         <v>0</v>
       </c>
       <c r="AB25" t="n">
-        <v>0</v>
+        <v>7.130438461899757e-10</v>
       </c>
       <c r="AC25" t="n">
-        <v>2.273736754432321e-13</v>
+        <v>-1.091393642127514e-09</v>
       </c>
     </row>
     <row r="26">
@@ -2721,76 +2721,76 @@
         <v>24</v>
       </c>
       <c r="B26" t="n">
-        <v>1289.800605426039</v>
+        <v>28434.17599074678</v>
       </c>
       <c r="C26" t="n">
-        <v>1.832942529274935</v>
+        <v>5.162249225908711</v>
       </c>
       <c r="D26" t="n">
-        <v>1.452941176470574</v>
+        <v>4.969863351536048</v>
       </c>
       <c r="E26" t="n">
-        <v>55.98396391222813</v>
+        <v>3.802722533226884</v>
       </c>
       <c r="F26" t="n">
-        <v>57.10148831016802</v>
+        <v>5.19923563880495</v>
       </c>
       <c r="G26" t="n">
-        <v>312.9256885708497</v>
+        <v>4041.292184661147</v>
       </c>
       <c r="H26" t="n">
-        <v>2301.224891075968</v>
+        <v>50541.90715940663</v>
       </c>
       <c r="I26" t="n">
-        <v>235.880643478786</v>
+        <v>103.7248810923845</v>
       </c>
       <c r="J26" t="n">
-        <v>0.627099814420246</v>
+        <v>0.2757574878739312</v>
       </c>
       <c r="K26" t="n">
-        <v>166.4090641347034</v>
+        <v>5331.317216568816</v>
       </c>
       <c r="L26" t="n">
-        <v>1314.299309575965</v>
+        <v>250913.8166759837</v>
       </c>
       <c r="M26" t="n">
-        <v>1147.890245441261</v>
+        <v>245582.4994594149</v>
       </c>
       <c r="N26" t="n">
-        <v>533.0184551962163</v>
+        <v>38465.10075366498</v>
       </c>
       <c r="O26" t="n">
-        <v>465.530705906943</v>
+        <v>37647.80955542903</v>
       </c>
       <c r="P26" t="n">
-        <v>1201.363392805065</v>
+        <v>247947.9369200711</v>
       </c>
       <c r="Q26" t="n">
-        <v>1049.253628746159</v>
+        <v>242679.6375397237</v>
       </c>
       <c r="R26" t="n">
-        <v>-1.647540906848555</v>
+        <v>19.94306232893676</v>
       </c>
       <c r="S26" t="n">
-        <v>-1.645695441642072</v>
+        <v>19.98851421519624</v>
       </c>
       <c r="T26" t="n">
-        <v>54.33642300537958</v>
+        <v>23.74578486216365</v>
       </c>
       <c r="U26" t="n">
-        <v>54.70793360722553</v>
+        <v>24.94292634794411</v>
       </c>
       <c r="V26" t="n">
-        <v>54.33826847058606</v>
+        <v>23.79123674842312</v>
       </c>
       <c r="W26" t="n">
-        <v>54.71006091298985</v>
+        <v>24.989372510672</v>
       </c>
       <c r="X26" t="n">
-        <v>54.33734573798282</v>
+        <v>23.76851080529338</v>
       </c>
       <c r="Y26" t="n">
-        <v>54.70899726010769</v>
+        <v>24.96614942930805</v>
       </c>
       <c r="Z26" t="n">
         <v>0</v>
@@ -2799,10 +2799,10 @@
         <v>0</v>
       </c>
       <c r="AB26" t="n">
-        <v>2.273736754432321e-13</v>
+        <v>-5.820766091346741e-11</v>
       </c>
       <c r="AC26" t="n">
-        <v>0</v>
+        <v>-2.328306436538696e-10</v>
       </c>
     </row>
     <row r="27">
@@ -2810,88 +2810,88 @@
         <v>25</v>
       </c>
       <c r="B27" t="n">
-        <v>1354.970550764645</v>
+        <v>27233.13588376297</v>
       </c>
       <c r="C27" t="n">
-        <v>1.86381147919721</v>
+        <v>5.230751938966827</v>
       </c>
       <c r="D27" t="n">
-        <v>1.452941176470603</v>
+        <v>4.96986335153602</v>
       </c>
       <c r="E27" t="n">
-        <v>57.10148831016802</v>
+        <v>5.19923563880495</v>
       </c>
       <c r="F27" t="n">
-        <v>58.26896956548119</v>
+        <v>6.830990895593999</v>
       </c>
       <c r="G27" t="n">
-        <v>268.8521014228305</v>
+        <v>4026.950228554961</v>
       </c>
       <c r="H27" t="n">
-        <v>2324.295266086307</v>
+        <v>49549.3654898609</v>
       </c>
       <c r="I27" t="n">
-        <v>235.880643478786</v>
+        <v>103.7248810923845</v>
       </c>
       <c r="J27" t="n">
-        <v>0.627099814420246</v>
+        <v>0.2757574878739312</v>
       </c>
       <c r="K27" t="n">
-        <v>172.2045514936872</v>
+        <v>7500.498764522452</v>
       </c>
       <c r="L27" t="n">
-        <v>1147.890245441261</v>
+        <v>245582.4994594149</v>
       </c>
       <c r="M27" t="n">
-        <v>975.685693947574</v>
+        <v>238082.0006948925</v>
       </c>
       <c r="N27" t="n">
-        <v>465.530705906943</v>
+        <v>37647.80955542903</v>
       </c>
       <c r="O27" t="n">
-        <v>395.6925774485659</v>
+        <v>36497.9827164684</v>
       </c>
       <c r="P27" t="n">
-        <v>1049.253628746159</v>
+        <v>242679.6375397237</v>
       </c>
       <c r="Q27" t="n">
-        <v>891.8463755188276</v>
+        <v>235267.7970154673</v>
       </c>
       <c r="R27" t="n">
-        <v>-2.393554702942493</v>
+        <v>19.74369070913916</v>
       </c>
       <c r="S27" t="n">
-        <v>-2.39142739717818</v>
+        <v>19.79013687186705</v>
       </c>
       <c r="T27" t="n">
-        <v>54.70793360722553</v>
+        <v>24.94292634794411</v>
       </c>
       <c r="U27" t="n">
-        <v>54.8839693415785</v>
+        <v>26.32235682136698</v>
       </c>
       <c r="V27" t="n">
-        <v>54.71006091298985</v>
+        <v>24.989372510672</v>
       </c>
       <c r="W27" t="n">
-        <v>54.88649155898671</v>
+        <v>26.37027974401116</v>
       </c>
       <c r="X27" t="n">
-        <v>54.70899726010769</v>
+        <v>24.96614942930805</v>
       </c>
       <c r="Y27" t="n">
-        <v>54.88523045028261</v>
+        <v>26.34631828268907</v>
       </c>
       <c r="Z27" t="n">
-        <v>0</v>
+        <v>-2.91038304567337e-11</v>
       </c>
       <c r="AA27" t="n">
-        <v>0</v>
+        <v>3.637978807091713e-12</v>
       </c>
       <c r="AB27" t="n">
-        <v>-6.821210263296962e-13</v>
+        <v>-2.328306436538696e-10</v>
       </c>
       <c r="AC27" t="n">
-        <v>6.821210263296962e-13</v>
+        <v>-1.455191522836685e-10</v>
       </c>
     </row>
     <row r="28">
@@ -2899,88 +2899,88 @@
         <v>26</v>
       </c>
       <c r="B28" t="n">
-        <v>1418.541039410279</v>
+        <v>26080.01117874081</v>
       </c>
       <c r="C28" t="n">
-        <v>1.897196030975709</v>
+        <v>5.312437295358902</v>
       </c>
       <c r="D28" t="n">
-        <v>1.452941176470574</v>
+        <v>4.969863351536048</v>
       </c>
       <c r="E28" t="n">
-        <v>58.26896956548119</v>
+        <v>6.830990895593999</v>
       </c>
       <c r="F28" t="n">
-        <v>59.4890582625445</v>
+        <v>8.708335164012681</v>
       </c>
       <c r="G28" t="n">
-        <v>221.5808411131931</v>
+        <v>3984.00963476891</v>
       </c>
       <c r="H28" t="n">
-        <v>2338.430966086148</v>
+        <v>48399.27944078912</v>
       </c>
       <c r="I28" t="n">
-        <v>235.880643478786</v>
+        <v>103.7248810923845</v>
       </c>
       <c r="J28" t="n">
-        <v>0.627099814420246</v>
+        <v>0.2757574878739312</v>
       </c>
       <c r="K28" t="n">
-        <v>173.4115577822015</v>
+        <v>9560.524336640436</v>
       </c>
       <c r="L28" t="n">
-        <v>975.685693947574</v>
+        <v>238082.0006948925</v>
       </c>
       <c r="M28" t="n">
-        <v>802.2741361653724</v>
+        <v>228521.476358252</v>
       </c>
       <c r="N28" t="n">
-        <v>395.6925774485659</v>
+        <v>36497.9827164684</v>
       </c>
       <c r="O28" t="n">
-        <v>325.364943576446</v>
+        <v>35032.35385338499</v>
       </c>
       <c r="P28" t="n">
-        <v>891.8463755188276</v>
+        <v>235267.7970154673</v>
       </c>
       <c r="Q28" t="n">
-        <v>733.3358323792658</v>
+        <v>225820.281065378</v>
       </c>
       <c r="R28" t="n">
-        <v>-3.385000223902685</v>
+        <v>19.49136592577299</v>
       </c>
       <c r="S28" t="n">
-        <v>-3.382478006494481</v>
+        <v>19.53928884841716</v>
       </c>
       <c r="T28" t="n">
-        <v>54.8839693415785</v>
+        <v>26.32235682136698</v>
       </c>
       <c r="U28" t="n">
-        <v>54.73473429997448</v>
+        <v>27.88564593394503</v>
       </c>
       <c r="V28" t="n">
-        <v>54.88649155898671</v>
+        <v>26.37027974401116</v>
       </c>
       <c r="W28" t="n">
-        <v>54.73782842149105</v>
+        <v>27.93559577048573</v>
       </c>
       <c r="X28" t="n">
-        <v>54.88523045028261</v>
+        <v>26.34631828268907</v>
       </c>
       <c r="Y28" t="n">
-        <v>54.73628136073276</v>
+        <v>27.91062085221538</v>
       </c>
       <c r="Z28" t="n">
-        <v>1.13686837721616e-13</v>
+        <v>2.91038304567337e-11</v>
       </c>
       <c r="AA28" t="n">
-        <v>0</v>
+        <v>3.637978807091713e-12</v>
       </c>
       <c r="AB28" t="n">
-        <v>2.273736754432321e-13</v>
+        <v>-6.111804395914078e-10</v>
       </c>
       <c r="AC28" t="n">
-        <v>2.273736754432321e-13</v>
+        <v>1.746229827404022e-10</v>
       </c>
     </row>
     <row r="29">
@@ -2988,88 +2988,88 @@
         <v>27</v>
       </c>
       <c r="B29" t="n">
-        <v>1480.758498790964</v>
+        <v>24899.5679429359</v>
       </c>
       <c r="C29" t="n">
-        <v>1.933395411990592</v>
+        <v>5.409029652929961</v>
       </c>
       <c r="D29" t="n">
-        <v>1.452941176470603</v>
+        <v>4.96986335153602</v>
       </c>
       <c r="E29" t="n">
-        <v>59.4890582625445</v>
+        <v>8.708335164012681</v>
       </c>
       <c r="F29" t="n">
-        <v>60.76472886656208</v>
+        <v>10.84393915685456</v>
       </c>
       <c r="G29" t="n">
-        <v>170.9368028516488</v>
+        <v>3925.368832167498</v>
       </c>
       <c r="H29" t="n">
-        <v>2343.142727691047</v>
+        <v>47084.13438855672</v>
       </c>
       <c r="I29" t="n">
-        <v>235.880643478786</v>
+        <v>103.7248810923845</v>
       </c>
       <c r="J29" t="n">
-        <v>0.627099814420246</v>
+        <v>0.2757574878739312</v>
       </c>
       <c r="K29" t="n">
-        <v>168.9112021143133</v>
+        <v>11520.3630668293</v>
       </c>
       <c r="L29" t="n">
-        <v>802.2741361653724</v>
+        <v>228521.476358252</v>
       </c>
       <c r="M29" t="n">
-        <v>633.3629340510589</v>
+        <v>217001.1132914227</v>
       </c>
       <c r="N29" t="n">
-        <v>325.364943576446</v>
+        <v>35032.35385338499</v>
       </c>
       <c r="O29" t="n">
-        <v>256.8624439096428</v>
+        <v>33266.28161410043</v>
       </c>
       <c r="P29" t="n">
-        <v>733.3358323792658</v>
+        <v>225820.281065378</v>
       </c>
       <c r="Q29" t="n">
-        <v>578.9389355869336</v>
+        <v>214436.0922915922</v>
       </c>
       <c r="R29" t="n">
-        <v>-4.754323962570024</v>
+        <v>19.17731076993235</v>
       </c>
       <c r="S29" t="n">
-        <v>-4.751229841053451</v>
+        <v>19.22726060647305</v>
       </c>
       <c r="T29" t="n">
-        <v>54.73473429997448</v>
+        <v>27.88564593394503</v>
       </c>
       <c r="U29" t="n">
-        <v>54.02728084682448</v>
+        <v>29.63850314785411</v>
       </c>
       <c r="V29" t="n">
-        <v>54.73782842149105</v>
+        <v>27.93559577048573</v>
       </c>
       <c r="W29" t="n">
-        <v>54.03123732435677</v>
+        <v>29.69113888533998</v>
       </c>
       <c r="X29" t="n">
-        <v>54.73628136073276</v>
+        <v>27.91062085221538</v>
       </c>
       <c r="Y29" t="n">
-        <v>54.02925908559062</v>
+        <v>29.66482101659705</v>
       </c>
       <c r="Z29" t="n">
-        <v>0</v>
+        <v>-2.91038304567337e-11</v>
       </c>
       <c r="AA29" t="n">
-        <v>0</v>
+        <v>3.637978807091713e-12</v>
       </c>
       <c r="AB29" t="n">
-        <v>0</v>
+        <v>1.309672370553017e-10</v>
       </c>
       <c r="AC29" t="n">
-        <v>-2.273736754432321e-13</v>
+        <v>7.130438461899757e-10</v>
       </c>
     </row>
     <row r="30">
@@ -3077,76 +3077,76 @@
         <v>28</v>
       </c>
       <c r="B30" t="n">
-        <v>1541.899667133067</v>
+        <v>23683.63500776632</v>
       </c>
       <c r="C30" t="n">
-        <v>1.97276281233556</v>
+        <v>5.522750734297738</v>
       </c>
       <c r="D30" t="n">
-        <v>1.452941176470574</v>
+        <v>4.969863351536048</v>
       </c>
       <c r="E30" t="n">
-        <v>60.76472886656208</v>
+        <v>10.84393915685456</v>
       </c>
       <c r="F30" t="n">
-        <v>62.09933634220274</v>
+        <v>13.25330219555589</v>
       </c>
       <c r="G30" t="n">
-        <v>116.722997895988</v>
+        <v>3850.153474338601</v>
       </c>
       <c r="H30" t="n">
-        <v>2337.880141179944</v>
+        <v>45594.73817853178</v>
       </c>
       <c r="I30" t="n">
-        <v>235.880643478786</v>
+        <v>103.7248810923845</v>
       </c>
       <c r="J30" t="n">
-        <v>0.627099814420246</v>
+        <v>0.2757574878739312</v>
       </c>
       <c r="K30" t="n">
-        <v>157.4242049804946</v>
+        <v>13367.65044769635</v>
       </c>
       <c r="L30" t="n">
-        <v>633.3629340510589</v>
+        <v>217001.1132914227</v>
       </c>
       <c r="M30" t="n">
-        <v>475.9387290705645</v>
+        <v>203633.4628437264</v>
       </c>
       <c r="N30" t="n">
-        <v>256.8624439096428</v>
+        <v>33266.28161410043</v>
       </c>
       <c r="O30" t="n">
-        <v>193.018534126058</v>
+        <v>31217.02012614336</v>
       </c>
       <c r="P30" t="n">
-        <v>578.9389355869336</v>
+        <v>214436.0922915922</v>
       </c>
       <c r="Q30" t="n">
-        <v>435.0419741968951</v>
+        <v>201226.4516512957</v>
       </c>
       <c r="R30" t="n">
-        <v>-6.737448019737601</v>
+        <v>18.79456399099955</v>
       </c>
       <c r="S30" t="n">
-        <v>-6.733491542205313</v>
+        <v>18.84719972848542</v>
       </c>
       <c r="T30" t="n">
-        <v>54.02728084682448</v>
+        <v>29.63850314785411</v>
       </c>
       <c r="U30" t="n">
-        <v>52.32926686159367</v>
+        <v>31.5894763817105</v>
       </c>
       <c r="V30" t="n">
-        <v>54.03123732435677</v>
+        <v>29.69113888533998</v>
       </c>
       <c r="W30" t="n">
-        <v>52.33458431072405</v>
+        <v>31.64561915197474</v>
       </c>
       <c r="X30" t="n">
-        <v>54.02925908559062</v>
+        <v>29.66482101659705</v>
       </c>
       <c r="Y30" t="n">
-        <v>52.33192558615886</v>
+        <v>31.61754776684262</v>
       </c>
       <c r="Z30" t="n">
         <v>0</v>
@@ -3155,10 +3155,10 @@
         <v>0</v>
       </c>
       <c r="AB30" t="n">
-        <v>-2.273736754432321e-13</v>
+        <v>3.492459654808044e-10</v>
       </c>
       <c r="AC30" t="n">
-        <v>4.547473508864641e-13</v>
+        <v>-1.455191522836685e-10</v>
       </c>
     </row>
     <row r="31">
@@ -3166,88 +3166,88 @@
         <v>29</v>
       </c>
       <c r="B31" t="n">
-        <v>1602.281798420868</v>
+        <v>22422.72714003907</v>
       </c>
       <c r="C31" t="n">
-        <v>2.015718451111918</v>
+        <v>5.656486579640865</v>
       </c>
       <c r="D31" t="n">
-        <v>1.452941176470603</v>
+        <v>4.96986335153602</v>
       </c>
       <c r="E31" t="n">
-        <v>62.09933634220274</v>
+        <v>13.25330219555589</v>
       </c>
       <c r="F31" t="n">
-        <v>63.49668638166201</v>
+        <v>15.95544088205149</v>
       </c>
       <c r="G31" t="n">
-        <v>58.71662390607074</v>
+        <v>3757.292928014294</v>
       </c>
       <c r="H31" t="n">
-        <v>2322.020670602627</v>
+        <v>43919.83505851075</v>
       </c>
       <c r="I31" t="n">
-        <v>235.880643478786</v>
+        <v>103.7248810923845</v>
       </c>
       <c r="J31" t="n">
-        <v>0.627099814420246</v>
+        <v>0.2757574878739312</v>
       </c>
       <c r="K31" t="n">
-        <v>137.4716295446562</v>
+        <v>15086.85463483783</v>
       </c>
       <c r="L31" t="n">
-        <v>475.9387290705645</v>
+        <v>203633.4628437264</v>
       </c>
       <c r="M31" t="n">
-        <v>338.4670995259085</v>
+        <v>188546.6082088886</v>
       </c>
       <c r="N31" t="n">
-        <v>193.018534126058</v>
+        <v>31217.02012614336</v>
       </c>
       <c r="O31" t="n">
-        <v>137.2664576551056</v>
+        <v>28904.204549573</v>
       </c>
       <c r="P31" t="n">
-        <v>435.0419741968951</v>
+        <v>201226.4516512957</v>
       </c>
       <c r="Q31" t="n">
-        <v>309.3830911092271</v>
+        <v>186317.928354822</v>
       </c>
       <c r="R31" t="n">
-        <v>-9.770069480609068</v>
+        <v>18.33617418615462</v>
       </c>
       <c r="S31" t="n">
-        <v>-9.764752031478686</v>
+        <v>18.39231695641885</v>
       </c>
       <c r="T31" t="n">
-        <v>52.32926686159367</v>
+        <v>31.5894763817105</v>
       </c>
       <c r="U31" t="n">
-        <v>48.8528010217336</v>
+        <v>33.750367290112</v>
       </c>
       <c r="V31" t="n">
-        <v>52.33458431072405</v>
+        <v>31.64561915197474</v>
       </c>
       <c r="W31" t="n">
-        <v>48.86035150209675</v>
+        <v>33.81108023003203</v>
       </c>
       <c r="X31" t="n">
-        <v>52.33192558615886</v>
+        <v>31.61754776684262</v>
       </c>
       <c r="Y31" t="n">
-        <v>48.85657626191518</v>
+        <v>33.78072376007201</v>
       </c>
       <c r="Z31" t="n">
-        <v>0</v>
+        <v>-2.91038304567337e-11</v>
       </c>
       <c r="AA31" t="n">
         <v>0</v>
       </c>
       <c r="AB31" t="n">
-        <v>4.547473508864641e-13</v>
+        <v>0</v>
       </c>
       <c r="AC31" t="n">
-        <v>-4.547473508864641e-13</v>
+        <v>-2.037268131971359e-10</v>
       </c>
     </row>
     <row r="32">
@@ -3255,88 +3255,88 @@
         <v>30</v>
       </c>
       <c r="B32" t="n">
-        <v>1654.224287071587</v>
+        <v>21105.55354486355</v>
       </c>
       <c r="C32" t="n">
-        <v>2.062766731572732</v>
+        <v>5.814033583378821</v>
       </c>
       <c r="D32" t="n">
-        <v>1.452941176470574</v>
+        <v>4.969863351536048</v>
       </c>
       <c r="E32" t="n">
-        <v>63.49668638166201</v>
+        <v>15.95544088205149</v>
       </c>
       <c r="F32" t="n">
-        <v>64.96112347479303</v>
+        <v>18.97384502774857</v>
       </c>
       <c r="G32" t="n">
-        <v>0</v>
+        <v>3645.46976783431</v>
       </c>
       <c r="H32" t="n">
-        <v>2291.656242144128</v>
+        <v>42045.57470845997</v>
       </c>
       <c r="I32" t="n">
-        <v>235.880643478786</v>
+        <v>103.7248810923845</v>
       </c>
       <c r="J32" t="n">
-        <v>0.627099814420246</v>
+        <v>0.2757574878739312</v>
       </c>
       <c r="K32" t="n">
-        <v>110.3055723423113</v>
+        <v>16658.23447632405</v>
       </c>
       <c r="L32" t="n">
-        <v>338.4670995259085</v>
+        <v>188546.6082088886</v>
       </c>
       <c r="M32" t="n">
-        <v>228.1615271835973</v>
+        <v>171888.3737325645</v>
       </c>
       <c r="N32" t="n">
-        <v>137.2664576551056</v>
+        <v>28904.204549573</v>
       </c>
       <c r="O32" t="n">
-        <v>92.53166601285611</v>
+        <v>26350.49636403525</v>
       </c>
       <c r="P32" t="n">
-        <v>309.3830911092271</v>
+        <v>186317.928354822</v>
       </c>
       <c r="Q32" t="n">
-        <v>208.5559236071626</v>
+        <v>169856.5994178464</v>
       </c>
       <c r="R32" t="n">
-        <v>-14.6438853599284</v>
+        <v>17.7949264080605</v>
       </c>
       <c r="S32" t="n">
-        <v>-14.63633487956526</v>
+        <v>17.85563934798055</v>
       </c>
       <c r="T32" t="n">
-        <v>48.8528010217336</v>
+        <v>33.750367290112</v>
       </c>
       <c r="U32" t="n">
-        <v>42.21957833955089</v>
+        <v>36.13696187998781</v>
       </c>
       <c r="V32" t="n">
-        <v>48.86035150209675</v>
+        <v>33.81108023003203</v>
       </c>
       <c r="W32" t="n">
-        <v>42.23087940833368</v>
+        <v>36.20367621647335</v>
       </c>
       <c r="X32" t="n">
-        <v>48.85657626191518</v>
+        <v>33.78072376007201</v>
       </c>
       <c r="Y32" t="n">
-        <v>42.22522887394229</v>
+        <v>36.17031904823058</v>
       </c>
       <c r="Z32" t="n">
-        <v>0</v>
+        <v>-2.91038304567337e-11</v>
       </c>
       <c r="AA32" t="n">
         <v>0</v>
       </c>
       <c r="AB32" t="n">
-        <v>-9.094947017729282e-13</v>
+        <v>-2.91038304567337e-11</v>
       </c>
       <c r="AC32" t="n">
-        <v>1.364242052659392e-12</v>
+        <v>0</v>
       </c>
     </row>
     <row r="33">
@@ -3344,88 +3344,88 @@
         <v>31</v>
       </c>
       <c r="B33" t="n">
-        <v>1585.878388007719</v>
+        <v>19905.62045451007</v>
       </c>
       <c r="C33" t="n">
-        <v>2.114519087332646</v>
+        <v>6.000470880018844</v>
       </c>
       <c r="D33" t="n">
-        <v>1.452941176470603</v>
+        <v>4.96986335153602</v>
       </c>
       <c r="E33" t="n">
-        <v>64.96112347479303</v>
+        <v>18.97384502774857</v>
       </c>
       <c r="F33" t="n">
-        <v>66.49764270734632</v>
+        <v>22.33783428860198</v>
       </c>
       <c r="G33" t="n">
-        <v>0</v>
+        <v>3477.774280522214</v>
       </c>
       <c r="H33" t="n">
-        <v>2230.583521959219</v>
+        <v>39954.76747270864</v>
       </c>
       <c r="I33" t="n">
-        <v>235.880643478786</v>
+        <v>103.7248810923845</v>
       </c>
       <c r="J33" t="n">
-        <v>0.627099814420246</v>
+        <v>0.2757574878739312</v>
       </c>
       <c r="K33" t="n">
-        <v>137.9880194254681</v>
+        <v>17999.19693950302</v>
       </c>
       <c r="L33" t="n">
-        <v>228.1615271835973</v>
+        <v>171888.3737325645</v>
       </c>
       <c r="M33" t="n">
-        <v>90.17350775812912</v>
+        <v>153889.1767930615</v>
       </c>
       <c r="N33" t="n">
-        <v>92.53166601285611</v>
+        <v>26350.49636403525</v>
       </c>
       <c r="O33" t="n">
-        <v>36.57016590868411</v>
+        <v>23591.21856524789</v>
       </c>
       <c r="P33" t="n">
-        <v>208.5559236071626</v>
+        <v>169856.5994178464</v>
       </c>
       <c r="Q33" t="n">
-        <v>82.42502330492051</v>
+        <v>152070.1586132297</v>
       </c>
       <c r="R33" t="n">
-        <v>-22.74154513524214</v>
+        <v>17.16311685223924</v>
       </c>
       <c r="S33" t="n">
-        <v>-22.73024406645934</v>
+        <v>17.22983118872478</v>
       </c>
       <c r="T33" t="n">
-        <v>42.21957833955089</v>
+        <v>36.13696187998781</v>
       </c>
       <c r="U33" t="n">
-        <v>7.381379986900178</v>
+        <v>38.76365852875936</v>
       </c>
       <c r="V33" t="n">
-        <v>42.23087940833368</v>
+        <v>36.20367621647335</v>
       </c>
       <c r="W33" t="n">
-        <v>7.410342261437521</v>
+        <v>38.83835526828337</v>
       </c>
       <c r="X33" t="n">
-        <v>42.22522887394229</v>
+        <v>36.17031904823058</v>
       </c>
       <c r="Y33" t="n">
-        <v>7.395861124168849</v>
+        <v>38.80100689852136</v>
       </c>
       <c r="Z33" t="n">
-        <v>0</v>
+        <v>2.91038304567337e-11</v>
       </c>
       <c r="AA33" t="n">
         <v>0</v>
       </c>
       <c r="AB33" t="n">
-        <v>-2.273736754432321e-13</v>
+        <v>1.600710675120354e-10</v>
       </c>
       <c r="AC33" t="n">
-        <v>-4.547473508864641e-13</v>
+        <v>2.619344741106033e-10</v>
       </c>
     </row>
     <row r="34">
@@ -3433,88 +3433,88 @@
         <v>32</v>
       </c>
       <c r="B34" t="n">
-        <v>1506.725839315156</v>
+        <v>18658.99122719847</v>
       </c>
       <c r="C34" t="n">
-        <v>2.171724892562904</v>
+        <v>6.222742491942144</v>
       </c>
       <c r="D34" t="n">
-        <v>1.452941176470574</v>
+        <v>4.96986335153602</v>
       </c>
       <c r="E34" t="n">
-        <v>66.49764270734632</v>
+        <v>22.33783428860198</v>
       </c>
       <c r="F34" t="n">
-        <v>68.11203362096626</v>
+        <v>26.08453721064944</v>
       </c>
       <c r="G34" t="n">
-        <v>0</v>
+        <v>3281.391874984613</v>
       </c>
       <c r="H34" t="n">
-        <v>2155.369734706901</v>
+        <v>37625.81352029299</v>
       </c>
       <c r="I34" t="n">
-        <v>235.880643478786</v>
+        <v>103.7248810923845</v>
       </c>
       <c r="J34" t="n">
-        <v>0.627099814420246</v>
+        <v>0.2757574878739312</v>
       </c>
       <c r="K34" t="n">
-        <v>158.6254474534414</v>
+        <v>19117.62215044658</v>
       </c>
       <c r="L34" t="n">
-        <v>90.17350775812912</v>
+        <v>153889.1767930615</v>
       </c>
       <c r="M34" t="n">
-        <v>-68.45193969531223</v>
+        <v>134771.5546426149</v>
       </c>
       <c r="N34" t="n">
-        <v>36.57016590868411</v>
+        <v>23591.21856524789</v>
       </c>
       <c r="O34" t="n">
-        <v>-27.76091175407487</v>
+        <v>20660.48612520442</v>
       </c>
       <c r="P34" t="n">
-        <v>82.42502330492051</v>
+        <v>152070.1586132297</v>
       </c>
       <c r="Q34" t="n">
-        <v>-62.56995945845842</v>
+        <v>133178.5127333144</v>
       </c>
       <c r="R34" t="n">
-        <v>-59.11626272044614</v>
+        <v>16.42582424015739</v>
       </c>
       <c r="S34" t="n">
-        <v>-59.0873004459088</v>
+        <v>16.50052097968138</v>
       </c>
       <c r="T34" t="n">
-        <v>7.381379986900178</v>
+        <v>38.76365852875936</v>
       </c>
       <c r="U34" t="n">
-        <v>146.1416023912028</v>
+        <v>41.65349380046887</v>
       </c>
       <c r="V34" t="n">
-        <v>7.410342261437521</v>
+        <v>38.83835526828337</v>
       </c>
       <c r="W34" t="n">
-        <v>146.1027985663146</v>
+        <v>41.73906667523217</v>
       </c>
       <c r="X34" t="n">
-        <v>7.395861124168849</v>
+        <v>38.80100689852136</v>
       </c>
       <c r="Y34" t="n">
-        <v>146.1222004787587</v>
+        <v>41.69628023785052</v>
       </c>
       <c r="Z34" t="n">
-        <v>5.684341886080801e-14</v>
+        <v>0</v>
       </c>
       <c r="AA34" t="n">
         <v>0</v>
       </c>
       <c r="AB34" t="n">
-        <v>2.273736754432321e-13</v>
+        <v>-7.275957614183426e-11</v>
       </c>
       <c r="AC34" t="n">
-        <v>2.273736754432321e-13</v>
+        <v>-6.257323548197746e-10</v>
       </c>
     </row>
     <row r="35">
@@ -3522,88 +3522,88 @@
         <v>33</v>
       </c>
       <c r="B35" t="n">
-        <v>1415.729792620841</v>
+        <v>17315.24147564516</v>
       </c>
       <c r="C35" t="n">
-        <v>2.235314028783751</v>
+        <v>6.49060361431328</v>
       </c>
       <c r="D35" t="n">
-        <v>1.452941176470574</v>
+        <v>4.969863351536048</v>
       </c>
       <c r="E35" t="n">
-        <v>68.11203362096626</v>
+        <v>26.08453721064944</v>
       </c>
       <c r="F35" t="n">
-        <v>69.81106817304104</v>
+        <v>30.26187762734655</v>
       </c>
       <c r="G35" t="n">
-        <v>0</v>
+        <v>3059.732215643516</v>
       </c>
       <c r="H35" t="n">
-        <v>2064.8336309714</v>
+        <v>35031.11543896214</v>
       </c>
       <c r="I35" t="n">
-        <v>235.880643478786</v>
+        <v>103.7248810923845</v>
       </c>
       <c r="J35" t="n">
-        <v>0.627099814420246</v>
+        <v>0.2757574878739312</v>
       </c>
       <c r="K35" t="n">
-        <v>170.7529888344459</v>
+        <v>19975.20349696155</v>
       </c>
       <c r="L35" t="n">
-        <v>-68.45193969531223</v>
+        <v>134771.5546426149</v>
       </c>
       <c r="M35" t="n">
-        <v>-239.2049285297582</v>
+        <v>114796.3511456534</v>
       </c>
       <c r="N35" t="n">
-        <v>-27.76091175407487</v>
+        <v>20660.48612520442</v>
       </c>
       <c r="O35" t="n">
-        <v>-97.01035414938235</v>
+        <v>17598.2864214799</v>
       </c>
       <c r="P35" t="n">
-        <v>-62.56995945845842</v>
+        <v>133178.5127333144</v>
       </c>
       <c r="Q35" t="n">
-        <v>-218.6503807925752</v>
+        <v>113439.4223865042</v>
       </c>
       <c r="R35" t="n">
-        <v>78.02956877023651</v>
+        <v>15.56895658981942</v>
       </c>
       <c r="S35" t="n">
-        <v>77.9907649453483</v>
+        <v>15.65452946458272</v>
       </c>
       <c r="T35" t="n">
-        <v>146.1416023912028</v>
+        <v>41.65349380046887</v>
       </c>
       <c r="U35" t="n">
-        <v>91.46240925641786</v>
+        <v>44.83698400602207</v>
       </c>
       <c r="V35" t="n">
-        <v>146.1027985663146</v>
+        <v>41.73906667523217</v>
       </c>
       <c r="W35" t="n">
-        <v>91.45106806975494</v>
+        <v>44.93790078514814</v>
       </c>
       <c r="X35" t="n">
-        <v>146.1222004787587</v>
+        <v>41.69628023785052</v>
       </c>
       <c r="Y35" t="n">
-        <v>91.4567386630864</v>
+        <v>44.88744239558511</v>
       </c>
       <c r="Z35" t="n">
-        <v>-5.684341886080801e-14</v>
+        <v>-1.455191522836685e-11</v>
       </c>
       <c r="AA35" t="n">
-        <v>0</v>
+        <v>3.637978807091713e-12</v>
       </c>
       <c r="AB35" t="n">
-        <v>-6.821210263296962e-13</v>
+        <v>2.91038304567337e-11</v>
       </c>
       <c r="AC35" t="n">
-        <v>0</v>
+        <v>-8.731149137020111e-11</v>
       </c>
     </row>
     <row r="36">
@@ -3611,88 +3611,88 @@
         <v>34</v>
       </c>
       <c r="B36" t="n">
-        <v>1311.61927633851</v>
+        <v>15849.28692062707</v>
       </c>
       <c r="C36" t="n">
-        <v>2.306456683259107</v>
+        <v>6.818233486606601</v>
       </c>
       <c r="D36" t="n">
-        <v>1.452941176470603</v>
+        <v>4.96986335153602</v>
       </c>
       <c r="E36" t="n">
-        <v>69.81106817304104</v>
+        <v>30.26187762734655</v>
       </c>
       <c r="F36" t="n">
-        <v>71.60275058215227</v>
+        <v>34.9332733700486</v>
       </c>
       <c r="G36" t="n">
-        <v>0</v>
+        <v>2809.36739249391</v>
       </c>
       <c r="H36" t="n">
-        <v>1957.586533314994</v>
+        <v>32134.63501960603</v>
       </c>
       <c r="I36" t="n">
-        <v>235.880643478786</v>
+        <v>103.7248810923845</v>
       </c>
       <c r="J36" t="n">
-        <v>0.627099814420246</v>
+        <v>0.2757574878739312</v>
       </c>
       <c r="K36" t="n">
-        <v>172.6284539388755</v>
+        <v>20505.44635991991</v>
       </c>
       <c r="L36" t="n">
-        <v>-239.2049285297582</v>
+        <v>114796.3511456534</v>
       </c>
       <c r="M36" t="n">
-        <v>-411.8333824686336</v>
+        <v>94290.90478573347</v>
       </c>
       <c r="N36" t="n">
-        <v>-97.01035414938235</v>
+        <v>17598.2864214799</v>
       </c>
       <c r="O36" t="n">
-        <v>-167.0203976539302</v>
+        <v>14454.80046011599</v>
       </c>
       <c r="P36" t="n">
-        <v>-218.6503807925752</v>
+        <v>113439.4223865042</v>
       </c>
       <c r="Q36" t="n">
-        <v>-376.445111115922</v>
+        <v>93176.35681314484</v>
       </c>
       <c r="R36" t="n">
-        <v>21.65134108337683</v>
+        <v>14.57510637867552</v>
       </c>
       <c r="S36" t="n">
-        <v>21.6399998967139</v>
+        <v>14.6760231578016</v>
       </c>
       <c r="T36" t="n">
-        <v>91.46240925641786</v>
+        <v>44.83698400602207</v>
       </c>
       <c r="U36" t="n">
-        <v>83.27192799312226</v>
+        <v>48.35313008729139</v>
       </c>
       <c r="V36" t="n">
-        <v>91.45106806975494</v>
+        <v>44.93790078514814</v>
       </c>
       <c r="W36" t="n">
-        <v>83.26517439941307</v>
+        <v>48.47676567360037</v>
       </c>
       <c r="X36" t="n">
-        <v>91.4567386630864</v>
+        <v>44.88744239558511</v>
       </c>
       <c r="Y36" t="n">
-        <v>83.26855119626767</v>
+        <v>48.41494788044588</v>
       </c>
       <c r="Z36" t="n">
-        <v>5.684341886080801e-14</v>
+        <v>1.455191522836685e-11</v>
       </c>
       <c r="AA36" t="n">
         <v>0</v>
       </c>
       <c r="AB36" t="n">
-        <v>4.547473508864641e-13</v>
+        <v>7.275957614183426e-11</v>
       </c>
       <c r="AC36" t="n">
-        <v>-2.273736754432321e-13</v>
+        <v>0</v>
       </c>
     </row>
     <row r="37">
@@ -3700,76 +3700,76 @@
         <v>35</v>
       </c>
       <c r="B37" t="n">
-        <v>1192.820363765317</v>
+        <v>14226.74377712723</v>
       </c>
       <c r="C37" t="n">
-        <v>2.386649274574875</v>
+        <v>7.227149932025194</v>
       </c>
       <c r="D37" t="n">
-        <v>1.452941176470603</v>
+        <v>4.96986335153602</v>
       </c>
       <c r="E37" t="n">
-        <v>71.60275058215227</v>
+        <v>34.9332733700486</v>
       </c>
       <c r="F37" t="n">
-        <v>73.49665601649136</v>
+        <v>40.18542571287773</v>
       </c>
       <c r="G37" t="n">
-        <v>0</v>
+        <v>2525.691864102421</v>
       </c>
       <c r="H37" t="n">
-        <v>1831.977535277769</v>
+        <v>28887.9534107982</v>
       </c>
       <c r="I37" t="n">
-        <v>235.880643478786</v>
+        <v>103.7248810923845</v>
       </c>
       <c r="J37" t="n">
-        <v>0.627099814420246</v>
+        <v>0.2757574878739312</v>
       </c>
       <c r="K37" t="n">
-        <v>162.1475986995352</v>
+        <v>20611.92529406253</v>
       </c>
       <c r="L37" t="n">
-        <v>-411.8333824686336</v>
+        <v>94290.90478573347</v>
       </c>
       <c r="M37" t="n">
-        <v>-573.9809811681688</v>
+        <v>73678.97949167092</v>
       </c>
       <c r="N37" t="n">
-        <v>-167.0203976539302</v>
+        <v>14454.80046011599</v>
       </c>
       <c r="O37" t="n">
-        <v>-232.7798954661041</v>
+        <v>11294.99127277674</v>
       </c>
       <c r="P37" t="n">
-        <v>-376.445111115922</v>
+        <v>93176.35681314484</v>
       </c>
       <c r="Q37" t="n">
-        <v>-524.6595915539555</v>
+        <v>72808.07091993278</v>
       </c>
       <c r="R37" t="n">
-        <v>11.66917741096999</v>
+        <v>13.41985671724279</v>
       </c>
       <c r="S37" t="n">
-        <v>11.66242381726081</v>
+        <v>13.54349230355177</v>
       </c>
       <c r="T37" t="n">
-        <v>83.27192799312226</v>
+        <v>48.35313008729139</v>
       </c>
       <c r="U37" t="n">
-        <v>80.79658932543379</v>
+        <v>52.25085621766326</v>
       </c>
       <c r="V37" t="n">
-        <v>83.26517439941307</v>
+        <v>48.47676567360037</v>
       </c>
       <c r="W37" t="n">
-        <v>80.79160776271021</v>
+        <v>52.41049009615671</v>
       </c>
       <c r="X37" t="n">
-        <v>83.26855119626767</v>
+        <v>48.41494788044588</v>
       </c>
       <c r="Y37" t="n">
-        <v>80.794098544072</v>
+        <v>52.33067315690999</v>
       </c>
       <c r="Z37" t="n">
         <v>0</v>
@@ -3778,10 +3778,10 @@
         <v>0</v>
       </c>
       <c r="AB37" t="n">
-        <v>2.273736754432321e-13</v>
+        <v>1.746229827404022e-10</v>
       </c>
       <c r="AC37" t="n">
-        <v>4.547473508864641e-13</v>
+        <v>4.365574568510056e-11</v>
       </c>
     </row>
     <row r="38">
@@ -3789,88 +3789,88 @@
         <v>36</v>
       </c>
       <c r="B38" t="n">
-        <v>1057.358948017519</v>
+        <v>12592.16970954293</v>
       </c>
       <c r="C38" t="n">
-        <v>2.477841156573934</v>
+        <v>7.751879343416413</v>
       </c>
       <c r="D38" t="n">
-        <v>1.452941176470574</v>
+        <v>4.969863351536048</v>
       </c>
       <c r="E38" t="n">
-        <v>73.49665601649136</v>
+        <v>40.18542571287773</v>
       </c>
       <c r="F38" t="n">
-        <v>75.50440019361704</v>
+        <v>46.14212652486975</v>
       </c>
       <c r="G38" t="n">
-        <v>0</v>
+        <v>2202.281457511585</v>
       </c>
       <c r="H38" t="n">
-        <v>1686.018401400583</v>
+        <v>25406.37935533922</v>
       </c>
       <c r="I38" t="n">
-        <v>235.880643478786</v>
+        <v>103.7248810923845</v>
       </c>
       <c r="J38" t="n">
-        <v>0.627099814420246</v>
+        <v>0.2757574878739312</v>
       </c>
       <c r="K38" t="n">
-        <v>136.7248873064391</v>
+        <v>20263.23377038481</v>
       </c>
       <c r="L38" t="n">
-        <v>-573.9809811681688</v>
+        <v>73678.97949167092</v>
       </c>
       <c r="M38" t="n">
-        <v>-710.705868474608</v>
+        <v>53415.74572128611</v>
       </c>
       <c r="N38" t="n">
-        <v>-232.7798954661041</v>
+        <v>11294.99127277674</v>
       </c>
       <c r="O38" t="n">
-        <v>-288.2291281393431</v>
+        <v>8188.636513606864</v>
       </c>
       <c r="P38" t="n">
-        <v>-524.6595915539555</v>
+        <v>72808.07091993278</v>
       </c>
       <c r="Q38" t="n">
-        <v>-649.6358989282235</v>
+        <v>52784.35490757768</v>
       </c>
       <c r="R38" t="n">
-        <v>7.299933308942432</v>
+        <v>12.06543050478553</v>
       </c>
       <c r="S38" t="n">
-        <v>7.294951746218859</v>
+        <v>12.22506438327898</v>
       </c>
       <c r="T38" t="n">
-        <v>80.79658932543379</v>
+        <v>52.25085621766326</v>
       </c>
       <c r="U38" t="n">
-        <v>80.16804687479198</v>
+        <v>56.61382987526372</v>
       </c>
       <c r="V38" t="n">
-        <v>80.79160776271021</v>
+        <v>52.41049009615671</v>
       </c>
       <c r="W38" t="n">
-        <v>80.16390971775454</v>
+        <v>56.83689455089893</v>
       </c>
       <c r="X38" t="n">
-        <v>80.794098544072</v>
+        <v>52.33067315690999</v>
       </c>
       <c r="Y38" t="n">
-        <v>80.16597829627327</v>
+        <v>56.72536221308133</v>
       </c>
       <c r="Z38" t="n">
-        <v>1.13686837721616e-13</v>
+        <v>0</v>
       </c>
       <c r="AA38" t="n">
-        <v>2.273736754432321e-13</v>
+        <v>9.094947017729282e-13</v>
       </c>
       <c r="AB38" t="n">
-        <v>0</v>
+        <v>-5.820766091346741e-11</v>
       </c>
       <c r="AC38" t="n">
-        <v>0</v>
+        <v>-1.455191522836685e-10</v>
       </c>
     </row>
     <row r="39">
@@ -3878,88 +3878,88 @@
         <v>37</v>
       </c>
       <c r="B39" t="n">
-        <v>752.7981282190626</v>
+        <v>10908.87500949798</v>
       </c>
       <c r="C39" t="n">
-        <v>2.329469504482719</v>
+        <v>8.452100486961212</v>
       </c>
       <c r="D39" t="n">
-        <v>1.313262907348445</v>
+        <v>4.969863351536048</v>
       </c>
       <c r="E39" t="n">
-        <v>75.50440019361704</v>
+        <v>46.14212652486975</v>
       </c>
       <c r="F39" t="n">
-        <v>77.42894111287163</v>
+        <v>52.99100361566175</v>
       </c>
       <c r="G39" t="n">
-        <v>0</v>
+        <v>1829.709586425171</v>
       </c>
       <c r="H39" t="n">
-        <v>1288.483752140515</v>
+        <v>21605.23008997263</v>
       </c>
       <c r="I39" t="n">
-        <v>235.880643478786</v>
+        <v>103.7248810923845</v>
       </c>
       <c r="J39" t="n">
-        <v>0.627099814420246</v>
+        <v>0.2757574878739312</v>
       </c>
       <c r="K39" t="n">
-        <v>50.16205425814419</v>
+        <v>19276.16110586184</v>
       </c>
       <c r="L39" t="n">
-        <v>-710.705868474608</v>
+        <v>53415.74572128611</v>
       </c>
       <c r="M39" t="n">
-        <v>-760.867922732752</v>
+        <v>34139.58461542427</v>
       </c>
       <c r="N39" t="n">
-        <v>-288.2291281393431</v>
+        <v>8188.636513606864</v>
       </c>
       <c r="O39" t="n">
-        <v>-308.5725160383834</v>
+        <v>5233.60004370081</v>
       </c>
       <c r="P39" t="n">
-        <v>-649.6358989282235</v>
+        <v>52784.35490757768</v>
       </c>
       <c r="Q39" t="n">
-        <v>-695.4875974375062</v>
+        <v>33736.04405226387</v>
       </c>
       <c r="R39" t="n">
-        <v>4.66364668117494</v>
+        <v>10.47170335039397</v>
       </c>
       <c r="S39" t="n">
-        <v>4.659509524137484</v>
+        <v>10.69476802602918</v>
       </c>
       <c r="T39" t="n">
-        <v>80.16804687479198</v>
+        <v>56.61382987526372</v>
       </c>
       <c r="U39" t="n">
-        <v>80.48750158525041</v>
+        <v>61.57808879749265</v>
       </c>
       <c r="V39" t="n">
-        <v>80.16390971775454</v>
+        <v>56.83689455089893</v>
       </c>
       <c r="W39" t="n">
-        <v>80.4836013939441</v>
+        <v>61.93406036741318</v>
       </c>
       <c r="X39" t="n">
-        <v>80.16597829627327</v>
+        <v>56.72536221308133</v>
       </c>
       <c r="Y39" t="n">
-        <v>80.48555148959726</v>
+        <v>61.75607458245291</v>
       </c>
       <c r="Z39" t="n">
-        <v>-5.684341886080801e-14</v>
+        <v>0</v>
       </c>
       <c r="AA39" t="n">
-        <v>0</v>
+        <v>-9.094947017729282e-13</v>
       </c>
       <c r="AB39" t="n">
-        <v>3.410605131648481e-13</v>
+        <v>-2.91038304567337e-11</v>
       </c>
       <c r="AC39" t="n">
-        <v>3.410605131648481e-13</v>
+        <v>0</v>
       </c>
     </row>
     <row r="40">
@@ -3967,79 +3967,79 @@
         <v>38</v>
       </c>
       <c r="B40" t="n">
-        <v>469.417064307613</v>
+        <v>9002.673756139786</v>
       </c>
       <c r="C40" t="n">
-        <v>2.427547636618971</v>
+        <v>9.442301189058211</v>
       </c>
       <c r="D40" t="n">
-        <v>1.313262907348445</v>
+        <v>4.96986335153602</v>
       </c>
       <c r="E40" t="n">
-        <v>77.42894111287163</v>
+        <v>52.99100361566175</v>
       </c>
       <c r="F40" t="n">
-        <v>79.47126890591167</v>
+        <v>61.04216222470259</v>
       </c>
       <c r="G40" t="n">
-        <v>0</v>
+        <v>1384.527423904875</v>
       </c>
       <c r="H40" t="n">
-        <v>950.1749686251959</v>
+        <v>17192.24892393892</v>
       </c>
       <c r="I40" t="n">
-        <v>235.880643478786</v>
+        <v>103.7248810923845</v>
       </c>
       <c r="J40" t="n">
-        <v>0.627099814420246</v>
+        <v>0.2757574878739312</v>
       </c>
       <c r="K40" t="n">
-        <v>-81.20583545405279</v>
+        <v>17151.04193850708</v>
       </c>
       <c r="L40" t="n">
-        <v>-760.867922732752</v>
+        <v>34139.58461542427</v>
       </c>
       <c r="M40" t="n">
-        <v>-679.6620872786992</v>
+        <v>16988.54267691719</v>
       </c>
       <c r="N40" t="n">
-        <v>-308.5725160383834</v>
+        <v>5233.60004370081</v>
       </c>
       <c r="O40" t="n">
-        <v>-275.6392194511682</v>
+        <v>2604.344449350938</v>
       </c>
       <c r="P40" t="n">
-        <v>-695.4875974375062</v>
+        <v>33736.04405226387</v>
       </c>
       <c r="Q40" t="n">
-        <v>-621.2596667935147</v>
+        <v>16787.73279137393</v>
       </c>
       <c r="R40" t="n">
-        <v>3.05856047237878</v>
+        <v>8.587085181830894</v>
       </c>
       <c r="S40" t="n">
-        <v>3.054660281072478</v>
+        <v>8.943056751751429</v>
       </c>
       <c r="T40" t="n">
-        <v>80.48750158525041</v>
+        <v>61.57808879749265</v>
       </c>
       <c r="U40" t="n">
-        <v>81.34836274417577</v>
+        <v>67.33198867413753</v>
       </c>
       <c r="V40" t="n">
-        <v>80.4836013939441</v>
+        <v>61.93406036741318</v>
       </c>
       <c r="W40" t="n">
-        <v>81.34407773645361</v>
+        <v>68.0701682356539</v>
       </c>
       <c r="X40" t="n">
-        <v>80.48555148959726</v>
+        <v>61.75607458245291</v>
       </c>
       <c r="Y40" t="n">
-        <v>81.34622024031469</v>
+        <v>67.70107845489571</v>
       </c>
       <c r="Z40" t="n">
-        <v>1.13686837721616e-13</v>
+        <v>0</v>
       </c>
       <c r="AA40" t="n">
         <v>0</v>
@@ -4048,7 +4048,7 @@
         <v>0</v>
       </c>
       <c r="AC40" t="n">
-        <v>4.547473508864641e-13</v>
+        <v>1.455191522836685e-11</v>
       </c>
     </row>
     <row r="41">
@@ -4056,88 +4056,88 @@
         <v>39</v>
       </c>
       <c r="B41" t="n">
-        <v>166.4484618013738</v>
+        <v>6690.059058780809</v>
       </c>
       <c r="C41" t="n">
-        <v>2.541323463701519</v>
+        <v>10.97954524865555</v>
       </c>
       <c r="D41" t="n">
-        <v>1.313262907348445</v>
+        <v>4.96986335153602</v>
       </c>
       <c r="E41" t="n">
-        <v>79.47126890591167</v>
+        <v>61.04216222470259</v>
       </c>
       <c r="F41" t="n">
-        <v>81.64783755837817</v>
+        <v>70.88331657802578</v>
       </c>
       <c r="G41" t="n">
-        <v>0</v>
+        <v>836.8507439282687</v>
       </c>
       <c r="H41" t="n">
-        <v>590.4354452794314</v>
+        <v>11834.74036012506</v>
       </c>
       <c r="I41" t="n">
-        <v>235.880643478786</v>
+        <v>103.7248810923845</v>
       </c>
       <c r="J41" t="n">
-        <v>0.627099814420246</v>
+        <v>0.2757574878739312</v>
       </c>
       <c r="K41" t="n">
-        <v>-242.0070555295134</v>
+        <v>12961.16114100649</v>
       </c>
       <c r="L41" t="n">
-        <v>-679.6620872786992</v>
+        <v>16988.54267691719</v>
       </c>
       <c r="M41" t="n">
-        <v>-437.6550317491859</v>
+        <v>4027.381535910695</v>
       </c>
       <c r="N41" t="n">
-        <v>-275.6392194511682</v>
+        <v>2604.344449350938</v>
       </c>
       <c r="O41" t="n">
-        <v>-177.4924533796378</v>
+        <v>617.3977926145926</v>
       </c>
       <c r="P41" t="n">
-        <v>-621.2596667935147</v>
+        <v>16787.73279137393</v>
       </c>
       <c r="Q41" t="n">
-        <v>-400.0479418877918</v>
+        <v>3979.776627082105</v>
       </c>
       <c r="R41" t="n">
-        <v>1.877093838264099</v>
+        <v>6.289826449434942</v>
       </c>
       <c r="S41" t="n">
-        <v>1.872808830541948</v>
+        <v>7.028006010951305</v>
       </c>
       <c r="T41" t="n">
-        <v>81.34836274417577</v>
+        <v>67.33198867413753</v>
       </c>
       <c r="U41" t="n">
-        <v>82.52806689231191</v>
+        <v>73.66845424044205</v>
       </c>
       <c r="V41" t="n">
-        <v>81.34407773645361</v>
+        <v>68.0701682356539</v>
       </c>
       <c r="W41" t="n">
-        <v>82.52189340264339</v>
+        <v>76.9458025337189</v>
       </c>
       <c r="X41" t="n">
-        <v>81.34622024031469</v>
+        <v>67.70107845489571</v>
       </c>
       <c r="Y41" t="n">
-        <v>82.52498014747765</v>
+        <v>75.30712838708047</v>
       </c>
       <c r="Z41" t="n">
         <v>0</v>
       </c>
       <c r="AA41" t="n">
-        <v>0</v>
+        <v>4.547473508864641e-13</v>
       </c>
       <c r="AB41" t="n">
-        <v>-2.842170943040401e-14</v>
+        <v>0</v>
       </c>
       <c r="AC41" t="n">
-        <v>2.842170943040401e-14</v>
+        <v>0</v>
       </c>
     </row>
     <row r="42">
@@ -4145,76 +4145,76 @@
         <v>40</v>
       </c>
       <c r="B42" t="n">
-        <v>-160.2326016131221</v>
+        <v>3159.329195747139</v>
       </c>
       <c r="C42" t="n">
-        <v>2.675285503802047</v>
+        <v>13.82038689721892</v>
       </c>
       <c r="D42" t="n">
-        <v>1.313262907348445</v>
+        <v>4.969863351536048</v>
       </c>
       <c r="E42" t="n">
-        <v>81.64783755837817</v>
+        <v>70.88331657802578</v>
       </c>
       <c r="F42" t="n">
-        <v>83.97975317326198</v>
+        <v>83.95181749179723</v>
       </c>
       <c r="G42" t="n">
-        <v>0</v>
+        <v>144.2747922248728</v>
       </c>
       <c r="H42" t="n">
-        <v>206.0937437855559</v>
+        <v>4621.078153359055</v>
       </c>
       <c r="I42" t="n">
-        <v>235.880643478786</v>
+        <v>103.7248810923845</v>
       </c>
       <c r="J42" t="n">
-        <v>0.627099814420246</v>
+        <v>0.2757574878739312</v>
       </c>
       <c r="K42" t="n">
-        <v>-437.6533876265188</v>
+        <v>4027.351777569043</v>
       </c>
       <c r="L42" t="n">
-        <v>-437.6550317491859</v>
+        <v>4027.381535910695</v>
       </c>
       <c r="M42" t="n">
-        <v>-0.001644122667055575</v>
+        <v>0.02975834165275151</v>
       </c>
       <c r="N42" t="n">
-        <v>-177.4924533796378</v>
+        <v>617.3977926145926</v>
       </c>
       <c r="O42" t="n">
-        <v>-0.0006667794145230007</v>
+        <v>0.004561955276513209</v>
       </c>
       <c r="P42" t="n">
-        <v>-400.0479418877918</v>
+        <v>3979.776627082105</v>
       </c>
       <c r="Q42" t="n">
-        <v>-0.001502845486633374</v>
+        <v>0.02940658875111118</v>
       </c>
       <c r="R42" t="n">
-        <v>0.8802293339337466</v>
+        <v>2.785137662416258</v>
       </c>
       <c r="S42" t="n">
-        <v>0.8740558442652112</v>
+        <v>6.062485955693124</v>
       </c>
       <c r="T42" t="n">
-        <v>82.52806689231191</v>
+        <v>73.66845424044205</v>
       </c>
       <c r="U42" t="n">
-        <v>83.97975317326198</v>
+        <v>83.95181749179723</v>
       </c>
       <c r="V42" t="n">
-        <v>82.52189340264339</v>
+        <v>76.9458025337189</v>
       </c>
       <c r="W42" t="n">
-        <v>83.97975317326198</v>
+        <v>83.95181749179723</v>
       </c>
       <c r="X42" t="n">
-        <v>82.52498014747765</v>
+        <v>75.30712838708047</v>
       </c>
       <c r="Y42" t="n">
-        <v>83.97975317326198</v>
+        <v>83.95181749179723</v>
       </c>
       <c r="Z42" t="n">
         <v>0</v>

</xml_diff>